<commit_message>
Updating the GESS model with the latest data
</commit_message>
<xml_diff>
--- a/Market Fundamentals/Transelectrica_data/Cons_Prod_final/Weekly_Production_2026.xlsx
+++ b/Market Fundamentals/Transelectrica_data/Cons_Prod_final/Weekly_Production_2026.xlsx
@@ -36703,7 +36703,7 @@
         <v>1</v>
       </c>
       <c r="C2018">
-        <v>7476.9</v>
+        <v>6199.8</v>
       </c>
       <c r="D2018" t="s">
         <v>2020</v>
@@ -36717,7 +36717,7 @@
         <v>2</v>
       </c>
       <c r="C2019">
-        <v>7504.7</v>
+        <v>6198.6</v>
       </c>
       <c r="D2019" t="s">
         <v>2021</v>
@@ -36731,7 +36731,7 @@
         <v>3</v>
       </c>
       <c r="C2020">
-        <v>7478.6</v>
+        <v>6229.9</v>
       </c>
       <c r="D2020" t="s">
         <v>2022</v>
@@ -36745,7 +36745,7 @@
         <v>4</v>
       </c>
       <c r="C2021">
-        <v>7486.8</v>
+        <v>6215.8</v>
       </c>
       <c r="D2021" t="s">
         <v>2023</v>
@@ -36759,7 +36759,7 @@
         <v>5</v>
       </c>
       <c r="C2022">
-        <v>7402.3</v>
+        <v>5914.3</v>
       </c>
       <c r="D2022" t="s">
         <v>2024</v>
@@ -36773,7 +36773,7 @@
         <v>6</v>
       </c>
       <c r="C2023">
-        <v>7375.7</v>
+        <v>5888.9</v>
       </c>
       <c r="D2023" t="s">
         <v>2025</v>
@@ -36787,7 +36787,7 @@
         <v>7</v>
       </c>
       <c r="C2024">
-        <v>7354.1</v>
+        <v>5865.2</v>
       </c>
       <c r="D2024" t="s">
         <v>2026</v>
@@ -36801,7 +36801,7 @@
         <v>8</v>
       </c>
       <c r="C2025">
-        <v>7321.1</v>
+        <v>5882.9</v>
       </c>
       <c r="D2025" t="s">
         <v>2027</v>
@@ -36815,7 +36815,7 @@
         <v>9</v>
       </c>
       <c r="C2026">
-        <v>7421.4</v>
+        <v>5880.4</v>
       </c>
       <c r="D2026" t="s">
         <v>2028</v>
@@ -36829,7 +36829,7 @@
         <v>10</v>
       </c>
       <c r="C2027">
-        <v>7398.1</v>
+        <v>5816</v>
       </c>
       <c r="D2027" t="s">
         <v>2029</v>
@@ -36843,7 +36843,7 @@
         <v>11</v>
       </c>
       <c r="C2028">
-        <v>7390.2</v>
+        <v>5813.5</v>
       </c>
       <c r="D2028" t="s">
         <v>2030</v>
@@ -36857,7 +36857,7 @@
         <v>12</v>
       </c>
       <c r="C2029">
-        <v>7378.4</v>
+        <v>5798.8</v>
       </c>
       <c r="D2029" t="s">
         <v>2031</v>
@@ -36871,7 +36871,7 @@
         <v>13</v>
       </c>
       <c r="C2030">
-        <v>7385.3</v>
+        <v>5803</v>
       </c>
       <c r="D2030" t="s">
         <v>2032</v>
@@ -36885,7 +36885,7 @@
         <v>14</v>
       </c>
       <c r="C2031">
-        <v>7357.5</v>
+        <v>5789.7</v>
       </c>
       <c r="D2031" t="s">
         <v>2033</v>
@@ -36899,7 +36899,7 @@
         <v>15</v>
       </c>
       <c r="C2032">
-        <v>7363.7</v>
+        <v>5781.9</v>
       </c>
       <c r="D2032" t="s">
         <v>2034</v>
@@ -36913,7 +36913,7 @@
         <v>16</v>
       </c>
       <c r="C2033">
-        <v>7360</v>
+        <v>5742.5</v>
       </c>
       <c r="D2033" t="s">
         <v>2035</v>
@@ -36927,7 +36927,7 @@
         <v>17</v>
       </c>
       <c r="C2034">
-        <v>7438.6</v>
+        <v>5803.1</v>
       </c>
       <c r="D2034" t="s">
         <v>2036</v>
@@ -36941,7 +36941,7 @@
         <v>18</v>
       </c>
       <c r="C2035">
-        <v>7446.3</v>
+        <v>5795.5</v>
       </c>
       <c r="D2035" t="s">
         <v>2037</v>
@@ -36955,7 +36955,7 @@
         <v>19</v>
       </c>
       <c r="C2036">
-        <v>7451.8</v>
+        <v>5796.8</v>
       </c>
       <c r="D2036" t="s">
         <v>2038</v>
@@ -36969,7 +36969,7 @@
         <v>20</v>
       </c>
       <c r="C2037">
-        <v>7462.7</v>
+        <v>5812.1</v>
       </c>
       <c r="D2037" t="s">
         <v>2039</v>
@@ -36983,7 +36983,7 @@
         <v>21</v>
       </c>
       <c r="C2038">
-        <v>7529.9</v>
+        <v>5789.3</v>
       </c>
       <c r="D2038" t="s">
         <v>2040</v>
@@ -36997,7 +36997,7 @@
         <v>22</v>
       </c>
       <c r="C2039">
-        <v>7521.8</v>
+        <v>5790.5</v>
       </c>
       <c r="D2039" t="s">
         <v>2041</v>
@@ -37011,7 +37011,7 @@
         <v>23</v>
       </c>
       <c r="C2040">
-        <v>7506.3</v>
+        <v>5800.8</v>
       </c>
       <c r="D2040" t="s">
         <v>2042</v>
@@ -37025,7 +37025,7 @@
         <v>24</v>
       </c>
       <c r="C2041">
-        <v>7491.4</v>
+        <v>5713.6</v>
       </c>
       <c r="D2041" t="s">
         <v>2043</v>
@@ -37039,7 +37039,7 @@
         <v>25</v>
       </c>
       <c r="C2042">
-        <v>7431.8</v>
+        <v>5747.5</v>
       </c>
       <c r="D2042" t="s">
         <v>2044</v>
@@ -37053,7 +37053,7 @@
         <v>26</v>
       </c>
       <c r="C2043">
-        <v>7435.5</v>
+        <v>5750.2</v>
       </c>
       <c r="D2043" t="s">
         <v>2045</v>
@@ -37067,7 +37067,7 @@
         <v>27</v>
       </c>
       <c r="C2044">
-        <v>7464.4</v>
+        <v>5779.5</v>
       </c>
       <c r="D2044" t="s">
         <v>2046</v>
@@ -37081,7 +37081,7 @@
         <v>28</v>
       </c>
       <c r="C2045">
-        <v>7451</v>
+        <v>5767</v>
       </c>
       <c r="D2045" t="s">
         <v>2047</v>
@@ -37095,7 +37095,7 @@
         <v>29</v>
       </c>
       <c r="C2046">
-        <v>7798.1</v>
+        <v>6287.3</v>
       </c>
       <c r="D2046" t="s">
         <v>2048</v>
@@ -37109,7 +37109,7 @@
         <v>30</v>
       </c>
       <c r="C2047">
-        <v>7793.9</v>
+        <v>6279.4</v>
       </c>
       <c r="D2047" t="s">
         <v>2049</v>
@@ -37123,7 +37123,7 @@
         <v>31</v>
       </c>
       <c r="C2048">
-        <v>7783.9</v>
+        <v>6420.2</v>
       </c>
       <c r="D2048" t="s">
         <v>2050</v>
@@ -37137,7 +37137,7 @@
         <v>32</v>
       </c>
       <c r="C2049">
-        <v>7740</v>
+        <v>6457.8</v>
       </c>
       <c r="D2049" t="s">
         <v>2051</v>
@@ -37151,7 +37151,7 @@
         <v>33</v>
       </c>
       <c r="C2050">
-        <v>7656.2</v>
+        <v>6396</v>
       </c>
       <c r="D2050" t="s">
         <v>2052</v>
@@ -37165,7 +37165,7 @@
         <v>34</v>
       </c>
       <c r="C2051">
-        <v>7596.6</v>
+        <v>6487.5</v>
       </c>
       <c r="D2051" t="s">
         <v>2053</v>
@@ -37179,7 +37179,7 @@
         <v>35</v>
       </c>
       <c r="C2052">
-        <v>7552.7</v>
+        <v>6596.5</v>
       </c>
       <c r="D2052" t="s">
         <v>2054</v>
@@ -37193,7 +37193,7 @@
         <v>36</v>
       </c>
       <c r="C2053">
-        <v>7489.5</v>
+        <v>6663.8</v>
       </c>
       <c r="D2053" t="s">
         <v>2055</v>
@@ -37207,7 +37207,7 @@
         <v>37</v>
       </c>
       <c r="C2054">
-        <v>7091.6</v>
+        <v>6479</v>
       </c>
       <c r="D2054" t="s">
         <v>2056</v>
@@ -37221,7 +37221,7 @@
         <v>38</v>
       </c>
       <c r="C2055">
-        <v>7015.6</v>
+        <v>6508.4</v>
       </c>
       <c r="D2055" t="s">
         <v>2057</v>
@@ -37235,7 +37235,7 @@
         <v>39</v>
       </c>
       <c r="C2056">
-        <v>6960.1</v>
+        <v>6553</v>
       </c>
       <c r="D2056" t="s">
         <v>2058</v>
@@ -37249,7 +37249,7 @@
         <v>40</v>
       </c>
       <c r="C2057">
-        <v>6890.3</v>
+        <v>6603</v>
       </c>
       <c r="D2057" t="s">
         <v>2059</v>
@@ -37263,7 +37263,7 @@
         <v>41</v>
       </c>
       <c r="C2058">
-        <v>6784.2</v>
+        <v>6507</v>
       </c>
       <c r="D2058" t="s">
         <v>2060</v>
@@ -37277,7 +37277,7 @@
         <v>42</v>
       </c>
       <c r="C2059">
-        <v>6705.9</v>
+        <v>6530.9</v>
       </c>
       <c r="D2059" t="s">
         <v>2061</v>
@@ -37291,7 +37291,7 @@
         <v>43</v>
       </c>
       <c r="C2060">
-        <v>6643.8</v>
+        <v>6566.7</v>
       </c>
       <c r="D2060" t="s">
         <v>2062</v>
@@ -37305,7 +37305,7 @@
         <v>44</v>
       </c>
       <c r="C2061">
-        <v>6614.6</v>
+        <v>6607.3</v>
       </c>
       <c r="D2061" t="s">
         <v>2063</v>
@@ -37319,7 +37319,7 @@
         <v>45</v>
       </c>
       <c r="C2062">
-        <v>6475.4</v>
+        <v>6173.8</v>
       </c>
       <c r="D2062" t="s">
         <v>2064</v>
@@ -37333,7 +37333,7 @@
         <v>46</v>
       </c>
       <c r="C2063">
-        <v>6440.8</v>
+        <v>6195.5</v>
       </c>
       <c r="D2063" t="s">
         <v>2065</v>
@@ -37347,7 +37347,7 @@
         <v>47</v>
       </c>
       <c r="C2064">
-        <v>6425.7</v>
+        <v>6253.5</v>
       </c>
       <c r="D2064" t="s">
         <v>2066</v>
@@ -37361,7 +37361,7 @@
         <v>48</v>
       </c>
       <c r="C2065">
-        <v>6408.3</v>
+        <v>6281.7</v>
       </c>
       <c r="D2065" t="s">
         <v>2067</v>
@@ -37375,7 +37375,7 @@
         <v>49</v>
       </c>
       <c r="C2066">
-        <v>6234.8</v>
+        <v>6371.9</v>
       </c>
       <c r="D2066" t="s">
         <v>2068</v>
@@ -37389,7 +37389,7 @@
         <v>50</v>
       </c>
       <c r="C2067">
-        <v>6249.8</v>
+        <v>6393.4</v>
       </c>
       <c r="D2067" t="s">
         <v>2069</v>
@@ -37403,7 +37403,7 @@
         <v>51</v>
       </c>
       <c r="C2068">
-        <v>6239.7</v>
+        <v>6381.2</v>
       </c>
       <c r="D2068" t="s">
         <v>2070</v>
@@ -37417,7 +37417,7 @@
         <v>52</v>
       </c>
       <c r="C2069">
-        <v>6253.3</v>
+        <v>6408.9</v>
       </c>
       <c r="D2069" t="s">
         <v>2071</v>
@@ -37431,7 +37431,7 @@
         <v>53</v>
       </c>
       <c r="C2070">
-        <v>6107.9</v>
+        <v>6210.9</v>
       </c>
       <c r="D2070" t="s">
         <v>2072</v>
@@ -37445,7 +37445,7 @@
         <v>54</v>
       </c>
       <c r="C2071">
-        <v>6095</v>
+        <v>6188.2</v>
       </c>
       <c r="D2071" t="s">
         <v>2073</v>
@@ -37459,7 +37459,7 @@
         <v>55</v>
       </c>
       <c r="C2072">
-        <v>6072</v>
+        <v>6185.8</v>
       </c>
       <c r="D2072" t="s">
         <v>2074</v>
@@ -37473,7 +37473,7 @@
         <v>56</v>
       </c>
       <c r="C2073">
-        <v>6092</v>
+        <v>6200.3</v>
       </c>
       <c r="D2073" t="s">
         <v>2075</v>
@@ -37487,7 +37487,7 @@
         <v>57</v>
       </c>
       <c r="C2074">
-        <v>5959.7</v>
+        <v>6211.4</v>
       </c>
       <c r="D2074" t="s">
         <v>2076</v>
@@ -37501,7 +37501,7 @@
         <v>58</v>
       </c>
       <c r="C2075">
-        <v>5977.3</v>
+        <v>6181.8</v>
       </c>
       <c r="D2075" t="s">
         <v>2077</v>
@@ -37515,7 +37515,7 @@
         <v>59</v>
       </c>
       <c r="C2076">
-        <v>5983.9</v>
+        <v>6151.8</v>
       </c>
       <c r="D2076" t="s">
         <v>2078</v>
@@ -37529,7 +37529,7 @@
         <v>60</v>
       </c>
       <c r="C2077">
-        <v>6005.6</v>
+        <v>6131.1</v>
       </c>
       <c r="D2077" t="s">
         <v>2079</v>
@@ -37543,7 +37543,7 @@
         <v>61</v>
       </c>
       <c r="C2078">
-        <v>6170.1</v>
+        <v>6093.5</v>
       </c>
       <c r="D2078" t="s">
         <v>2080</v>
@@ -37557,7 +37557,7 @@
         <v>62</v>
       </c>
       <c r="C2079">
-        <v>6167.1</v>
+        <v>6056.4</v>
       </c>
       <c r="D2079" t="s">
         <v>2081</v>
@@ -37571,7 +37571,7 @@
         <v>63</v>
       </c>
       <c r="C2080">
-        <v>6215.4</v>
+        <v>6029.3</v>
       </c>
       <c r="D2080" t="s">
         <v>2082</v>
@@ -37585,7 +37585,7 @@
         <v>64</v>
       </c>
       <c r="C2081">
-        <v>6214.6</v>
+        <v>5975</v>
       </c>
       <c r="D2081" t="s">
         <v>2083</v>
@@ -37599,7 +37599,7 @@
         <v>65</v>
       </c>
       <c r="C2082">
-        <v>6594.8</v>
+        <v>6412.7</v>
       </c>
       <c r="D2082" t="s">
         <v>2084</v>
@@ -37613,7 +37613,7 @@
         <v>66</v>
       </c>
       <c r="C2083">
-        <v>6658.2</v>
+        <v>6482.3</v>
       </c>
       <c r="D2083" t="s">
         <v>2085</v>
@@ -37627,7 +37627,7 @@
         <v>67</v>
       </c>
       <c r="C2084">
-        <v>6699.3</v>
+        <v>6462.5</v>
       </c>
       <c r="D2084" t="s">
         <v>2086</v>
@@ -37641,7 +37641,7 @@
         <v>68</v>
       </c>
       <c r="C2085">
-        <v>6726.3</v>
+        <v>6444.8</v>
       </c>
       <c r="D2085" t="s">
         <v>2087</v>
@@ -37655,7 +37655,7 @@
         <v>69</v>
       </c>
       <c r="C2086">
-        <v>6803.4</v>
+        <v>6948.9</v>
       </c>
       <c r="D2086" t="s">
         <v>2088</v>
@@ -37669,7 +37669,7 @@
         <v>70</v>
       </c>
       <c r="C2087">
-        <v>6864.7</v>
+        <v>7001.8</v>
       </c>
       <c r="D2087" t="s">
         <v>2089</v>
@@ -37683,7 +37683,7 @@
         <v>71</v>
       </c>
       <c r="C2088">
-        <v>6965.8</v>
+        <v>7050.2</v>
       </c>
       <c r="D2088" t="s">
         <v>2090</v>
@@ -37697,7 +37697,7 @@
         <v>72</v>
       </c>
       <c r="C2089">
-        <v>6976.8</v>
+        <v>7044</v>
       </c>
       <c r="D2089" t="s">
         <v>2091</v>
@@ -37711,7 +37711,7 @@
         <v>73</v>
       </c>
       <c r="C2090">
-        <v>7331.5</v>
+        <v>7211.5</v>
       </c>
       <c r="D2090" t="s">
         <v>2092</v>
@@ -37725,7 +37725,7 @@
         <v>74</v>
       </c>
       <c r="C2091">
-        <v>7337.9</v>
+        <v>7199.7</v>
       </c>
       <c r="D2091" t="s">
         <v>2093</v>
@@ -37739,7 +37739,7 @@
         <v>75</v>
       </c>
       <c r="C2092">
-        <v>7362.6</v>
+        <v>7226.1</v>
       </c>
       <c r="D2092" t="s">
         <v>2094</v>
@@ -37753,7 +37753,7 @@
         <v>76</v>
       </c>
       <c r="C2093">
-        <v>7434.4</v>
+        <v>7251.9</v>
       </c>
       <c r="D2093" t="s">
         <v>2095</v>
@@ -37767,7 +37767,7 @@
         <v>77</v>
       </c>
       <c r="C2094">
-        <v>7317</v>
+        <v>7221.2</v>
       </c>
       <c r="D2094" t="s">
         <v>2096</v>
@@ -37781,7 +37781,7 @@
         <v>78</v>
       </c>
       <c r="C2095">
-        <v>7320</v>
+        <v>7236.5</v>
       </c>
       <c r="D2095" t="s">
         <v>2097</v>
@@ -37795,7 +37795,7 @@
         <v>79</v>
       </c>
       <c r="C2096">
-        <v>7315.8</v>
+        <v>7232.7</v>
       </c>
       <c r="D2096" t="s">
         <v>2098</v>
@@ -37809,7 +37809,7 @@
         <v>80</v>
       </c>
       <c r="C2097">
-        <v>7270.1</v>
+        <v>7233.6</v>
       </c>
       <c r="D2097" t="s">
         <v>2099</v>
@@ -37823,7 +37823,7 @@
         <v>81</v>
       </c>
       <c r="C2098">
-        <v>7105.7</v>
+        <v>7044.5</v>
       </c>
       <c r="D2098" t="s">
         <v>2100</v>
@@ -37837,7 +37837,7 @@
         <v>82</v>
       </c>
       <c r="C2099">
-        <v>7136.4</v>
+        <v>7033.3</v>
       </c>
       <c r="D2099" t="s">
         <v>2101</v>
@@ -37851,7 +37851,7 @@
         <v>83</v>
       </c>
       <c r="C2100">
-        <v>7121.8</v>
+        <v>6968.3</v>
       </c>
       <c r="D2100" t="s">
         <v>2102</v>
@@ -37865,7 +37865,7 @@
         <v>84</v>
       </c>
       <c r="C2101">
-        <v>7127.3</v>
+        <v>6991.8</v>
       </c>
       <c r="D2101" t="s">
         <v>2103</v>
@@ -37879,7 +37879,7 @@
         <v>85</v>
       </c>
       <c r="C2102">
-        <v>6996.3</v>
+        <v>6902.8</v>
       </c>
       <c r="D2102" t="s">
         <v>2104</v>
@@ -37893,7 +37893,7 @@
         <v>86</v>
       </c>
       <c r="C2103">
-        <v>6943.2</v>
+        <v>6883</v>
       </c>
       <c r="D2103" t="s">
         <v>2105</v>
@@ -37907,7 +37907,7 @@
         <v>87</v>
       </c>
       <c r="C2104">
-        <v>6922.3</v>
+        <v>6830.2</v>
       </c>
       <c r="D2104" t="s">
         <v>2106</v>
@@ -37921,7 +37921,7 @@
         <v>88</v>
       </c>
       <c r="C2105">
-        <v>6893.3</v>
+        <v>6798.4</v>
       </c>
       <c r="D2105" t="s">
         <v>2107</v>
@@ -37935,7 +37935,7 @@
         <v>89</v>
       </c>
       <c r="C2106">
-        <v>6917.7</v>
+        <v>6591.3</v>
       </c>
       <c r="D2106" t="s">
         <v>2108</v>
@@ -37949,7 +37949,7 @@
         <v>90</v>
       </c>
       <c r="C2107">
-        <v>6884.8</v>
+        <v>6534</v>
       </c>
       <c r="D2107" t="s">
         <v>2109</v>
@@ -37963,7 +37963,7 @@
         <v>91</v>
       </c>
       <c r="C2108">
-        <v>6818.9</v>
+        <v>6486.2</v>
       </c>
       <c r="D2108" t="s">
         <v>2110</v>
@@ -37977,7 +37977,7 @@
         <v>92</v>
       </c>
       <c r="C2109">
-        <v>6743.1</v>
+        <v>6473.6</v>
       </c>
       <c r="D2109" t="s">
         <v>2111</v>
@@ -37991,7 +37991,7 @@
         <v>93</v>
       </c>
       <c r="C2110">
-        <v>6731.5</v>
+        <v>6364.6</v>
       </c>
       <c r="D2110" t="s">
         <v>2112</v>
@@ -38005,7 +38005,7 @@
         <v>94</v>
       </c>
       <c r="C2111">
-        <v>6681.6</v>
+        <v>6307.1</v>
       </c>
       <c r="D2111" t="s">
         <v>2113</v>
@@ -38019,7 +38019,7 @@
         <v>95</v>
       </c>
       <c r="C2112">
-        <v>6637.1</v>
+        <v>6239.6</v>
       </c>
       <c r="D2112" t="s">
         <v>2114</v>
@@ -38033,7 +38033,7 @@
         <v>96</v>
       </c>
       <c r="C2113">
-        <v>6604</v>
+        <v>6191.7</v>
       </c>
       <c r="D2113" t="s">
         <v>2115</v>
@@ -38047,7 +38047,7 @@
         <v>1</v>
       </c>
       <c r="C2114">
-        <v>7226.9</v>
+        <v>6004.1</v>
       </c>
       <c r="D2114" t="s">
         <v>2116</v>
@@ -38061,7 +38061,7 @@
         <v>2</v>
       </c>
       <c r="C2115">
-        <v>7254.7</v>
+        <v>5994.4</v>
       </c>
       <c r="D2115" t="s">
         <v>2117</v>
@@ -38075,7 +38075,7 @@
         <v>3</v>
       </c>
       <c r="C2116">
-        <v>7208.6</v>
+        <v>5983.9</v>
       </c>
       <c r="D2116" t="s">
         <v>2118</v>
@@ -38089,7 +38089,7 @@
         <v>4</v>
       </c>
       <c r="C2117">
-        <v>7216.8</v>
+        <v>5952.1</v>
       </c>
       <c r="D2117" t="s">
         <v>2119</v>
@@ -38103,7 +38103,7 @@
         <v>5</v>
       </c>
       <c r="C2118">
-        <v>7162.3</v>
+        <v>5589</v>
       </c>
       <c r="D2118" t="s">
         <v>2120</v>
@@ -38117,7 +38117,7 @@
         <v>6</v>
       </c>
       <c r="C2119">
-        <v>7165.7</v>
+        <v>5559</v>
       </c>
       <c r="D2119" t="s">
         <v>2121</v>
@@ -38131,7 +38131,7 @@
         <v>7</v>
       </c>
       <c r="C2120">
-        <v>7164.1</v>
+        <v>5519</v>
       </c>
       <c r="D2120" t="s">
         <v>2122</v>
@@ -38145,7 +38145,7 @@
         <v>8</v>
       </c>
       <c r="C2121">
-        <v>7141.1</v>
+        <v>5509</v>
       </c>
       <c r="D2121" t="s">
         <v>2123</v>
@@ -38159,7 +38159,7 @@
         <v>9</v>
       </c>
       <c r="C2122">
-        <v>7251.4</v>
+        <v>5399</v>
       </c>
       <c r="D2122" t="s">
         <v>2124</v>
@@ -38173,7 +38173,7 @@
         <v>10</v>
       </c>
       <c r="C2123">
-        <v>7248.1</v>
+        <v>5389</v>
       </c>
       <c r="D2123" t="s">
         <v>2125</v>
@@ -38187,7 +38187,7 @@
         <v>11</v>
       </c>
       <c r="C2124">
-        <v>7250.2</v>
+        <v>5379</v>
       </c>
       <c r="D2124" t="s">
         <v>2126</v>
@@ -38201,7 +38201,7 @@
         <v>12</v>
       </c>
       <c r="C2125">
-        <v>7248.4</v>
+        <v>5379</v>
       </c>
       <c r="D2125" t="s">
         <v>2127</v>
@@ -38215,7 +38215,7 @@
         <v>13</v>
       </c>
       <c r="C2126">
-        <v>7265.3</v>
+        <v>5361</v>
       </c>
       <c r="D2126" t="s">
         <v>2128</v>
@@ -38229,7 +38229,7 @@
         <v>14</v>
       </c>
       <c r="C2127">
-        <v>7267.5</v>
+        <v>5361</v>
       </c>
       <c r="D2127" t="s">
         <v>2129</v>
@@ -38243,7 +38243,7 @@
         <v>15</v>
       </c>
       <c r="C2128">
-        <v>7283.7</v>
+        <v>5371</v>
       </c>
       <c r="D2128" t="s">
         <v>2130</v>
@@ -38257,7 +38257,7 @@
         <v>16</v>
       </c>
       <c r="C2129">
-        <v>7280</v>
+        <v>5371</v>
       </c>
       <c r="D2129" t="s">
         <v>2131</v>
@@ -38271,7 +38271,7 @@
         <v>17</v>
       </c>
       <c r="C2130">
-        <v>7368.6</v>
+        <v>5375</v>
       </c>
       <c r="D2130" t="s">
         <v>2132</v>
@@ -38285,7 +38285,7 @@
         <v>18</v>
       </c>
       <c r="C2131">
-        <v>7376.3</v>
+        <v>5395</v>
       </c>
       <c r="D2131" t="s">
         <v>2133</v>
@@ -38299,7 +38299,7 @@
         <v>19</v>
       </c>
       <c r="C2132">
-        <v>7401.8</v>
+        <v>5425</v>
       </c>
       <c r="D2132" t="s">
         <v>2134</v>
@@ -38313,7 +38313,7 @@
         <v>20</v>
       </c>
       <c r="C2133">
-        <v>7452.7</v>
+        <v>5485</v>
       </c>
       <c r="D2133" t="s">
         <v>2135</v>
@@ -38327,7 +38327,7 @@
         <v>21</v>
       </c>
       <c r="C2134">
-        <v>7579.9</v>
+        <v>5626</v>
       </c>
       <c r="D2134" t="s">
         <v>2136</v>
@@ -38341,7 +38341,7 @@
         <v>22</v>
       </c>
       <c r="C2135">
-        <v>7671.8</v>
+        <v>5736</v>
       </c>
       <c r="D2135" t="s">
         <v>2137</v>
@@ -38355,7 +38355,7 @@
         <v>23</v>
       </c>
       <c r="C2136">
-        <v>7776.3</v>
+        <v>5856</v>
       </c>
       <c r="D2136" t="s">
         <v>2138</v>
@@ -38369,7 +38369,7 @@
         <v>24</v>
       </c>
       <c r="C2137">
-        <v>7921.4</v>
+        <v>6006</v>
       </c>
       <c r="D2137" t="s">
         <v>2139</v>
@@ -38383,7 +38383,7 @@
         <v>25</v>
       </c>
       <c r="C2138">
-        <v>8041.8</v>
+        <v>6239</v>
       </c>
       <c r="D2138" t="s">
         <v>2140</v>
@@ -38397,7 +38397,7 @@
         <v>26</v>
       </c>
       <c r="C2139">
-        <v>8225.5</v>
+        <v>6429</v>
       </c>
       <c r="D2139" t="s">
         <v>2141</v>
@@ -38411,7 +38411,7 @@
         <v>27</v>
       </c>
       <c r="C2140">
-        <v>8434.4</v>
+        <v>6619</v>
       </c>
       <c r="D2140" t="s">
         <v>2142</v>
@@ -38425,7 +38425,7 @@
         <v>28</v>
       </c>
       <c r="C2141">
-        <v>8611</v>
+        <v>6819</v>
       </c>
       <c r="D2141" t="s">
         <v>2143</v>
@@ -38439,7 +38439,7 @@
         <v>29</v>
       </c>
       <c r="C2142">
-        <v>9128.1</v>
+        <v>7096</v>
       </c>
       <c r="D2142" t="s">
         <v>2144</v>
@@ -38453,7 +38453,7 @@
         <v>30</v>
       </c>
       <c r="C2143">
-        <v>9273.9</v>
+        <v>7286</v>
       </c>
       <c r="D2143" t="s">
         <v>2145</v>
@@ -38467,7 +38467,7 @@
         <v>31</v>
       </c>
       <c r="C2144">
-        <v>9393.9</v>
+        <v>7466</v>
       </c>
       <c r="D2144" t="s">
         <v>2146</v>
@@ -38481,7 +38481,7 @@
         <v>32</v>
       </c>
       <c r="C2145">
-        <v>9450</v>
+        <v>7636</v>
       </c>
       <c r="D2145" t="s">
         <v>2147</v>
@@ -38495,7 +38495,7 @@
         <v>33</v>
       </c>
       <c r="C2146">
-        <v>9446.200000000001</v>
+        <v>7975</v>
       </c>
       <c r="D2146" t="s">
         <v>2148</v>
@@ -38509,7 +38509,7 @@
         <v>34</v>
       </c>
       <c r="C2147">
-        <v>9436.6</v>
+        <v>8105</v>
       </c>
       <c r="D2147" t="s">
         <v>2149</v>
@@ -38523,7 +38523,7 @@
         <v>35</v>
       </c>
       <c r="C2148">
-        <v>9412.700000000001</v>
+        <v>8215</v>
       </c>
       <c r="D2148" t="s">
         <v>2150</v>
@@ -38537,7 +38537,7 @@
         <v>36</v>
       </c>
       <c r="C2149">
-        <v>9339.5</v>
+        <v>8305</v>
       </c>
       <c r="D2149" t="s">
         <v>2151</v>
@@ -38551,7 +38551,7 @@
         <v>37</v>
       </c>
       <c r="C2150">
-        <v>8971.6</v>
+        <v>8381</v>
       </c>
       <c r="D2150" t="s">
         <v>2152</v>
@@ -38565,7 +38565,7 @@
         <v>38</v>
       </c>
       <c r="C2151">
-        <v>8925.6</v>
+        <v>8431</v>
       </c>
       <c r="D2151" t="s">
         <v>2153</v>
@@ -38579,7 +38579,7 @@
         <v>39</v>
       </c>
       <c r="C2152">
-        <v>8870.1</v>
+        <v>8461</v>
       </c>
       <c r="D2152" t="s">
         <v>2154</v>
@@ -38593,7 +38593,7 @@
         <v>40</v>
       </c>
       <c r="C2153">
-        <v>8810.299999999999</v>
+        <v>8461</v>
       </c>
       <c r="D2153" t="s">
         <v>2155</v>
@@ -38607,7 +38607,7 @@
         <v>41</v>
       </c>
       <c r="C2154">
-        <v>8714.200000000001</v>
+        <v>8386</v>
       </c>
       <c r="D2154" t="s">
         <v>2156</v>
@@ -38621,7 +38621,7 @@
         <v>42</v>
       </c>
       <c r="C2155">
-        <v>8645.9</v>
+        <v>8346</v>
       </c>
       <c r="D2155" t="s">
         <v>2157</v>
@@ -38635,7 +38635,7 @@
         <v>43</v>
       </c>
       <c r="C2156">
-        <v>8593.799999999999</v>
+        <v>8306</v>
       </c>
       <c r="D2156" t="s">
         <v>2158</v>
@@ -38649,7 +38649,7 @@
         <v>44</v>
       </c>
       <c r="C2157">
-        <v>8574.6</v>
+        <v>8246</v>
       </c>
       <c r="D2157" t="s">
         <v>2159</v>
@@ -38663,7 +38663,7 @@
         <v>45</v>
       </c>
       <c r="C2158">
-        <v>8445.4</v>
+        <v>8164</v>
       </c>
       <c r="D2158" t="s">
         <v>2160</v>
@@ -38677,7 +38677,7 @@
         <v>46</v>
       </c>
       <c r="C2159">
-        <v>8420.799999999999</v>
+        <v>8104</v>
       </c>
       <c r="D2159" t="s">
         <v>2161</v>
@@ -38691,7 +38691,7 @@
         <v>47</v>
       </c>
       <c r="C2160">
-        <v>8395.700000000001</v>
+        <v>8044</v>
       </c>
       <c r="D2160" t="s">
         <v>2162</v>
@@ -38705,7 +38705,7 @@
         <v>48</v>
       </c>
       <c r="C2161">
-        <v>8368.299999999999</v>
+        <v>7994</v>
       </c>
       <c r="D2161" t="s">
         <v>2163</v>
@@ -38719,7 +38719,7 @@
         <v>49</v>
       </c>
       <c r="C2162">
-        <v>8194.799999999999</v>
+        <v>7945</v>
       </c>
       <c r="D2162" t="s">
         <v>2164</v>
@@ -38733,7 +38733,7 @@
         <v>50</v>
       </c>
       <c r="C2163">
-        <v>8189.8</v>
+        <v>7915</v>
       </c>
       <c r="D2163" t="s">
         <v>2165</v>
@@ -38747,7 +38747,7 @@
         <v>51</v>
       </c>
       <c r="C2164">
-        <v>8169.7</v>
+        <v>7895</v>
       </c>
       <c r="D2164" t="s">
         <v>2166</v>
@@ -38761,7 +38761,7 @@
         <v>52</v>
       </c>
       <c r="C2165">
-        <v>8163.3</v>
+        <v>7875</v>
       </c>
       <c r="D2165" t="s">
         <v>2167</v>
@@ -38775,7 +38775,7 @@
         <v>53</v>
       </c>
       <c r="C2166">
-        <v>8007.9</v>
+        <v>7874</v>
       </c>
       <c r="D2166" t="s">
         <v>2168</v>
@@ -38789,7 +38789,7 @@
         <v>54</v>
       </c>
       <c r="C2167">
-        <v>7985</v>
+        <v>7874</v>
       </c>
       <c r="D2167" t="s">
         <v>2169</v>
@@ -38803,7 +38803,7 @@
         <v>55</v>
       </c>
       <c r="C2168">
-        <v>7962</v>
+        <v>7864</v>
       </c>
       <c r="D2168" t="s">
         <v>2170</v>
@@ -38817,7 +38817,7 @@
         <v>56</v>
       </c>
       <c r="C2169">
-        <v>7962</v>
+        <v>7864</v>
       </c>
       <c r="D2169" t="s">
         <v>2171</v>
@@ -38831,7 +38831,7 @@
         <v>57</v>
       </c>
       <c r="C2170">
-        <v>7829.7</v>
+        <v>7864</v>
       </c>
       <c r="D2170" t="s">
         <v>2172</v>
@@ -38845,7 +38845,7 @@
         <v>58</v>
       </c>
       <c r="C2171">
-        <v>7817.3</v>
+        <v>7854</v>
       </c>
       <c r="D2171" t="s">
         <v>2173</v>
@@ -38859,7 +38859,7 @@
         <v>59</v>
       </c>
       <c r="C2172">
-        <v>7793.9</v>
+        <v>7844</v>
       </c>
       <c r="D2172" t="s">
         <v>2174</v>
@@ -38873,7 +38873,7 @@
         <v>60</v>
       </c>
       <c r="C2173">
-        <v>7775.6</v>
+        <v>7844</v>
       </c>
       <c r="D2173" t="s">
         <v>2175</v>
@@ -38887,7 +38887,7 @@
         <v>61</v>
       </c>
       <c r="C2174">
-        <v>7870.1</v>
+        <v>7834</v>
       </c>
       <c r="D2174" t="s">
         <v>2176</v>
@@ -38901,7 +38901,7 @@
         <v>62</v>
       </c>
       <c r="C2175">
-        <v>7797.1</v>
+        <v>7834</v>
       </c>
       <c r="D2175" t="s">
         <v>2177</v>
@@ -38915,7 +38915,7 @@
         <v>63</v>
       </c>
       <c r="C2176">
-        <v>7755.4</v>
+        <v>7844</v>
       </c>
       <c r="D2176" t="s">
         <v>2178</v>
@@ -38929,7 +38929,7 @@
         <v>64</v>
       </c>
       <c r="C2177">
-        <v>7664.6</v>
+        <v>7864</v>
       </c>
       <c r="D2177" t="s">
         <v>2179</v>
@@ -38943,7 +38943,7 @@
         <v>65</v>
       </c>
       <c r="C2178">
-        <v>7964.8</v>
+        <v>7746</v>
       </c>
       <c r="D2178" t="s">
         <v>2180</v>
@@ -38957,7 +38957,7 @@
         <v>66</v>
       </c>
       <c r="C2179">
-        <v>7948.2</v>
+        <v>7796</v>
       </c>
       <c r="D2179" t="s">
         <v>2181</v>
@@ -38971,7 +38971,7 @@
         <v>67</v>
       </c>
       <c r="C2180">
-        <v>7919.3</v>
+        <v>7856</v>
       </c>
       <c r="D2180" t="s">
         <v>2182</v>
@@ -38985,7 +38985,7 @@
         <v>68</v>
       </c>
       <c r="C2181">
-        <v>7886.3</v>
+        <v>7926</v>
       </c>
       <c r="D2181" t="s">
         <v>2183</v>
@@ -38999,7 +38999,7 @@
         <v>69</v>
       </c>
       <c r="C2182">
-        <v>7913.4</v>
+        <v>8070</v>
       </c>
       <c r="D2182" t="s">
         <v>2184</v>
@@ -39013,7 +39013,7 @@
         <v>70</v>
       </c>
       <c r="C2183">
-        <v>7934.7</v>
+        <v>8140</v>
       </c>
       <c r="D2183" t="s">
         <v>2185</v>
@@ -39027,7 +39027,7 @@
         <v>71</v>
       </c>
       <c r="C2184">
-        <v>7995.8</v>
+        <v>8200</v>
       </c>
       <c r="D2184" t="s">
         <v>2186</v>
@@ -39041,7 +39041,7 @@
         <v>72</v>
       </c>
       <c r="C2185">
-        <v>7976.8</v>
+        <v>8260</v>
       </c>
       <c r="D2185" t="s">
         <v>2187</v>
@@ -39055,7 +39055,7 @@
         <v>73</v>
       </c>
       <c r="C2186">
-        <v>8301.5</v>
+        <v>8237</v>
       </c>
       <c r="D2186" t="s">
         <v>2188</v>
@@ -39069,7 +39069,7 @@
         <v>74</v>
       </c>
       <c r="C2187">
-        <v>8287.9</v>
+        <v>8277</v>
       </c>
       <c r="D2187" t="s">
         <v>2189</v>
@@ -39083,7 +39083,7 @@
         <v>75</v>
       </c>
       <c r="C2188">
-        <v>8302.6</v>
+        <v>8307</v>
       </c>
       <c r="D2188" t="s">
         <v>2190</v>
@@ -39097,7 +39097,7 @@
         <v>76</v>
       </c>
       <c r="C2189">
-        <v>8384.4</v>
+        <v>8337</v>
       </c>
       <c r="D2189" t="s">
         <v>2191</v>
@@ -39111,7 +39111,7 @@
         <v>77</v>
       </c>
       <c r="C2190">
-        <v>8307</v>
+        <v>8372</v>
       </c>
       <c r="D2190" t="s">
         <v>2192</v>
@@ -39125,7 +39125,7 @@
         <v>78</v>
       </c>
       <c r="C2191">
-        <v>8320</v>
+        <v>8362</v>
       </c>
       <c r="D2191" t="s">
         <v>2193</v>
@@ -39139,7 +39139,7 @@
         <v>79</v>
       </c>
       <c r="C2192">
-        <v>8315.799999999999</v>
+        <v>8332</v>
       </c>
       <c r="D2192" t="s">
         <v>2194</v>
@@ -39153,7 +39153,7 @@
         <v>80</v>
       </c>
       <c r="C2193">
-        <v>8270.1</v>
+        <v>8292</v>
       </c>
       <c r="D2193" t="s">
         <v>2195</v>
@@ -39167,7 +39167,7 @@
         <v>81</v>
       </c>
       <c r="C2194">
-        <v>8075.7</v>
+        <v>8307</v>
       </c>
       <c r="D2194" t="s">
         <v>2196</v>
@@ -39181,7 +39181,7 @@
         <v>82</v>
       </c>
       <c r="C2195">
-        <v>8076.4</v>
+        <v>8247</v>
       </c>
       <c r="D2195" t="s">
         <v>2197</v>
@@ -39195,7 +39195,7 @@
         <v>83</v>
       </c>
       <c r="C2196">
-        <v>8031.8</v>
+        <v>8157</v>
       </c>
       <c r="D2196" t="s">
         <v>2198</v>
@@ -39209,7 +39209,7 @@
         <v>84</v>
       </c>
       <c r="C2197">
-        <v>8017.3</v>
+        <v>8057</v>
       </c>
       <c r="D2197" t="s">
         <v>2199</v>
@@ -39223,7 +39223,7 @@
         <v>85</v>
       </c>
       <c r="C2198">
-        <v>7886.3</v>
+        <v>7880</v>
       </c>
       <c r="D2198" t="s">
         <v>2200</v>
@@ -39237,7 +39237,7 @@
         <v>86</v>
       </c>
       <c r="C2199">
-        <v>7813.2</v>
+        <v>7750</v>
       </c>
       <c r="D2199" t="s">
         <v>2201</v>
@@ -39251,7 +39251,7 @@
         <v>87</v>
       </c>
       <c r="C2200">
-        <v>7762.3</v>
+        <v>7630</v>
       </c>
       <c r="D2200" t="s">
         <v>2202</v>
@@ -39265,7 +39265,7 @@
         <v>88</v>
       </c>
       <c r="C2201">
-        <v>7663.3</v>
+        <v>7510</v>
       </c>
       <c r="D2201" t="s">
         <v>2203</v>
@@ -39279,7 +39279,7 @@
         <v>89</v>
       </c>
       <c r="C2202">
-        <v>7637.7</v>
+        <v>7440</v>
       </c>
       <c r="D2202" t="s">
         <v>2204</v>
@@ -39293,7 +39293,7 @@
         <v>90</v>
       </c>
       <c r="C2203">
-        <v>7574.8</v>
+        <v>7300</v>
       </c>
       <c r="D2203" t="s">
         <v>2205</v>
@@ -39307,7 +39307,7 @@
         <v>91</v>
       </c>
       <c r="C2204">
-        <v>7508.9</v>
+        <v>7140</v>
       </c>
       <c r="D2204" t="s">
         <v>2206</v>
@@ -39321,7 +39321,7 @@
         <v>92</v>
       </c>
       <c r="C2205">
-        <v>7373.1</v>
+        <v>7000</v>
       </c>
       <c r="D2205" t="s">
         <v>2207</v>
@@ -39335,7 +39335,7 @@
         <v>93</v>
       </c>
       <c r="C2206">
-        <v>7251.5</v>
+        <v>6954</v>
       </c>
       <c r="D2206" t="s">
         <v>2208</v>
@@ -39349,7 +39349,7 @@
         <v>94</v>
       </c>
       <c r="C2207">
-        <v>7151.6</v>
+        <v>6814</v>
       </c>
       <c r="D2207" t="s">
         <v>2209</v>
@@ -39363,7 +39363,7 @@
         <v>95</v>
       </c>
       <c r="C2208">
-        <v>7117.1</v>
+        <v>6694</v>
       </c>
       <c r="D2208" t="s">
         <v>2210</v>
@@ -39377,7 +39377,7 @@
         <v>96</v>
       </c>
       <c r="C2209">
-        <v>7084</v>
+        <v>6584</v>
       </c>
       <c r="D2209" t="s">
         <v>2211</v>
@@ -39391,7 +39391,7 @@
         <v>1</v>
       </c>
       <c r="C2210">
-        <v>6662.2</v>
+        <v>6272</v>
       </c>
       <c r="D2210" t="s">
         <v>2212</v>
@@ -39405,7 +39405,7 @@
         <v>2</v>
       </c>
       <c r="C2211">
-        <v>6626.3</v>
+        <v>6202</v>
       </c>
       <c r="D2211" t="s">
         <v>2213</v>
@@ -39419,7 +39419,7 @@
         <v>3</v>
       </c>
       <c r="C2212">
-        <v>6604.1</v>
+        <v>6152</v>
       </c>
       <c r="D2212" t="s">
         <v>2214</v>
@@ -39433,7 +39433,7 @@
         <v>4</v>
       </c>
       <c r="C2213">
-        <v>6512</v>
+        <v>6112</v>
       </c>
       <c r="D2213" t="s">
         <v>2215</v>
@@ -39447,7 +39447,7 @@
         <v>5</v>
       </c>
       <c r="C2214">
-        <v>7179</v>
+        <v>6096</v>
       </c>
       <c r="D2214" t="s">
         <v>2216</v>
@@ -39461,7 +39461,7 @@
         <v>6</v>
       </c>
       <c r="C2215">
-        <v>7075</v>
+        <v>6071</v>
       </c>
       <c r="D2215" t="s">
         <v>2217</v>
@@ -39475,7 +39475,7 @@
         <v>7</v>
       </c>
       <c r="C2216">
-        <v>7055.1</v>
+        <v>6035.8</v>
       </c>
       <c r="D2216" t="s">
         <v>2218</v>
@@ -39489,7 +39489,7 @@
         <v>8</v>
       </c>
       <c r="C2217">
-        <v>7005.6</v>
+        <v>5996.7</v>
       </c>
       <c r="D2217" t="s">
         <v>2219</v>
@@ -39503,7 +39503,7 @@
         <v>9</v>
       </c>
       <c r="C2218">
-        <v>6838.2</v>
+        <v>5965.2</v>
       </c>
       <c r="D2218" t="s">
         <v>2220</v>
@@ -39517,7 +39517,7 @@
         <v>10</v>
       </c>
       <c r="C2219">
-        <v>6854.7</v>
+        <v>5932.5</v>
       </c>
       <c r="D2219" t="s">
         <v>2221</v>
@@ -39531,7 +39531,7 @@
         <v>11</v>
       </c>
       <c r="C2220">
-        <v>6814.6</v>
+        <v>5937.3</v>
       </c>
       <c r="D2220" t="s">
         <v>2222</v>
@@ -39545,7 +39545,7 @@
         <v>12</v>
       </c>
       <c r="C2221">
-        <v>6808.4</v>
+        <v>5883.7</v>
       </c>
       <c r="D2221" t="s">
         <v>2223</v>
@@ -39559,7 +39559,7 @@
         <v>13</v>
       </c>
       <c r="C2222">
-        <v>6607.2</v>
+        <v>5934.3</v>
       </c>
       <c r="D2222" t="s">
         <v>2224</v>
@@ -39573,7 +39573,7 @@
         <v>14</v>
       </c>
       <c r="C2223">
-        <v>6598.6</v>
+        <v>5927.8</v>
       </c>
       <c r="D2223" t="s">
         <v>2225</v>
@@ -39587,7 +39587,7 @@
         <v>15</v>
       </c>
       <c r="C2224">
-        <v>6584.5</v>
+        <v>5912.4</v>
       </c>
       <c r="D2224" t="s">
         <v>2226</v>
@@ -39601,7 +39601,7 @@
         <v>16</v>
       </c>
       <c r="C2225">
-        <v>6570.9</v>
+        <v>5907.9</v>
       </c>
       <c r="D2225" t="s">
         <v>2227</v>
@@ -39615,7 +39615,7 @@
         <v>17</v>
       </c>
       <c r="C2226">
-        <v>6560.7</v>
+        <v>5886.8</v>
       </c>
       <c r="D2226" t="s">
         <v>2228</v>
@@ -39629,7 +39629,7 @@
         <v>18</v>
       </c>
       <c r="C2227">
-        <v>6574.4</v>
+        <v>5893.9</v>
       </c>
       <c r="D2227" t="s">
         <v>2229</v>
@@ -39643,7 +39643,7 @@
         <v>19</v>
       </c>
       <c r="C2228">
-        <v>6590.5</v>
+        <v>5884.1</v>
       </c>
       <c r="D2228" t="s">
         <v>2230</v>
@@ -39657,7 +39657,7 @@
         <v>20</v>
       </c>
       <c r="C2229">
-        <v>6620.7</v>
+        <v>5907.9</v>
       </c>
       <c r="D2229" t="s">
         <v>2231</v>
@@ -39671,7 +39671,7 @@
         <v>21</v>
       </c>
       <c r="C2230">
-        <v>6609.9</v>
+        <v>5836.6</v>
       </c>
       <c r="D2230" t="s">
         <v>2232</v>
@@ -39685,7 +39685,7 @@
         <v>22</v>
       </c>
       <c r="C2231">
-        <v>6650.4</v>
+        <v>5879.9</v>
       </c>
       <c r="D2231" t="s">
         <v>2233</v>
@@ -39699,7 +39699,7 @@
         <v>23</v>
       </c>
       <c r="C2232">
-        <v>6704</v>
+        <v>5904.8</v>
       </c>
       <c r="D2232" t="s">
         <v>2234</v>
@@ -39713,7 +39713,7 @@
         <v>24</v>
       </c>
       <c r="C2233">
-        <v>6725.2</v>
+        <v>5912.9</v>
       </c>
       <c r="D2233" t="s">
         <v>2235</v>
@@ -39727,7 +39727,7 @@
         <v>25</v>
       </c>
       <c r="C2234">
-        <v>7051.3</v>
+        <v>5917.8</v>
       </c>
       <c r="D2234" t="s">
         <v>2236</v>
@@ -39741,7 +39741,7 @@
         <v>26</v>
       </c>
       <c r="C2235">
-        <v>7064.8</v>
+        <v>6001.2</v>
       </c>
       <c r="D2235" t="s">
         <v>2237</v>
@@ -39755,7 +39755,7 @@
         <v>27</v>
       </c>
       <c r="C2236">
-        <v>7114.4</v>
+        <v>6098.7</v>
       </c>
       <c r="D2236" t="s">
         <v>2238</v>
@@ -39769,7 +39769,7 @@
         <v>28</v>
       </c>
       <c r="C2237">
-        <v>7129.6</v>
+        <v>6161</v>
       </c>
       <c r="D2237" t="s">
         <v>2239</v>
@@ -39783,7 +39783,7 @@
         <v>29</v>
       </c>
       <c r="C2238">
-        <v>7489.9</v>
+        <v>6918.9</v>
       </c>
       <c r="D2238" t="s">
         <v>2240</v>
@@ -39797,7 +39797,7 @@
         <v>30</v>
       </c>
       <c r="C2239">
-        <v>7521</v>
+        <v>6970.9</v>
       </c>
       <c r="D2239" t="s">
         <v>2241</v>
@@ -39811,7 +39811,7 @@
         <v>31</v>
       </c>
       <c r="C2240">
-        <v>7616.1</v>
+        <v>7099.7</v>
       </c>
       <c r="D2240" t="s">
         <v>2242</v>
@@ -39825,7 +39825,7 @@
         <v>32</v>
       </c>
       <c r="C2241">
-        <v>7656.9</v>
+        <v>7157.6</v>
       </c>
       <c r="D2241" t="s">
         <v>2243</v>
@@ -39839,7 +39839,7 @@
         <v>33</v>
       </c>
       <c r="C2242">
-        <v>7468.9</v>
+        <v>7105.7</v>
       </c>
       <c r="D2242" t="s">
         <v>2244</v>
@@ -39853,7 +39853,7 @@
         <v>34</v>
       </c>
       <c r="C2243">
-        <v>7532</v>
+        <v>7175.4</v>
       </c>
       <c r="D2243" t="s">
         <v>2245</v>
@@ -39867,7 +39867,7 @@
         <v>35</v>
       </c>
       <c r="C2244">
-        <v>7550.5</v>
+        <v>7204.1</v>
       </c>
       <c r="D2244" t="s">
         <v>2246</v>
@@ -39881,7 +39881,7 @@
         <v>36</v>
       </c>
       <c r="C2245">
-        <v>7559.7</v>
+        <v>7297.3</v>
       </c>
       <c r="D2245" t="s">
         <v>2247</v>
@@ -39895,7 +39895,7 @@
         <v>37</v>
       </c>
       <c r="C2246">
-        <v>7277.6</v>
+        <v>7242.8</v>
       </c>
       <c r="D2246" t="s">
         <v>2248</v>
@@ -39909,7 +39909,7 @@
         <v>38</v>
       </c>
       <c r="C2247">
-        <v>7272.2</v>
+        <v>7248.8</v>
       </c>
       <c r="D2247" t="s">
         <v>2249</v>
@@ -39923,7 +39923,7 @@
         <v>39</v>
       </c>
       <c r="C2248">
-        <v>7300.5</v>
+        <v>7285.1</v>
       </c>
       <c r="D2248" t="s">
         <v>2250</v>
@@ -39937,7 +39937,7 @@
         <v>40</v>
       </c>
       <c r="C2249">
-        <v>7310.2</v>
+        <v>7298</v>
       </c>
       <c r="D2249" t="s">
         <v>2251</v>
@@ -39951,7 +39951,7 @@
         <v>41</v>
       </c>
       <c r="C2250">
-        <v>6754.9</v>
+        <v>7274.4</v>
       </c>
       <c r="D2250" t="s">
         <v>2252</v>
@@ -39965,7 +39965,7 @@
         <v>42</v>
       </c>
       <c r="C2251">
-        <v>6744.7</v>
+        <v>7278.5</v>
       </c>
       <c r="D2251" t="s">
         <v>2253</v>
@@ -39979,7 +39979,7 @@
         <v>43</v>
       </c>
       <c r="C2252">
-        <v>6733.5</v>
+        <v>7320.1</v>
       </c>
       <c r="D2252" t="s">
         <v>2254</v>
@@ -39993,7 +39993,7 @@
         <v>44</v>
       </c>
       <c r="C2253">
-        <v>6733.2</v>
+        <v>7347.8</v>
       </c>
       <c r="D2253" t="s">
         <v>2255</v>
@@ -40007,7 +40007,7 @@
         <v>45</v>
       </c>
       <c r="C2254">
-        <v>6953.1</v>
+        <v>6990.9</v>
       </c>
       <c r="D2254" t="s">
         <v>2256</v>
@@ -40021,7 +40021,7 @@
         <v>46</v>
       </c>
       <c r="C2255">
-        <v>6909.6</v>
+        <v>7025.6</v>
       </c>
       <c r="D2255" t="s">
         <v>2257</v>
@@ -40035,7 +40035,7 @@
         <v>47</v>
       </c>
       <c r="C2256">
-        <v>6892.8</v>
+        <v>7054.3</v>
       </c>
       <c r="D2256" t="s">
         <v>2258</v>
@@ -40049,7 +40049,7 @@
         <v>48</v>
       </c>
       <c r="C2257">
-        <v>6871.7</v>
+        <v>7115.4</v>
       </c>
       <c r="D2257" t="s">
         <v>2259</v>
@@ -40063,7 +40063,7 @@
         <v>49</v>
       </c>
       <c r="C2258">
-        <v>6637.7</v>
+        <v>7113</v>
       </c>
       <c r="D2258" t="s">
         <v>2260</v>
@@ -40077,7 +40077,7 @@
         <v>50</v>
       </c>
       <c r="C2259">
-        <v>6609.4</v>
+        <v>7168</v>
       </c>
       <c r="D2259" t="s">
         <v>2261</v>
@@ -40091,7 +40091,7 @@
         <v>51</v>
       </c>
       <c r="C2260">
-        <v>6567.7</v>
+        <v>7214.6</v>
       </c>
       <c r="D2260" t="s">
         <v>2262</v>
@@ -40105,7 +40105,7 @@
         <v>52</v>
       </c>
       <c r="C2261">
-        <v>6518</v>
+        <v>7279.2</v>
       </c>
       <c r="D2261" t="s">
         <v>2263</v>
@@ -40119,7 +40119,7 @@
         <v>53</v>
       </c>
       <c r="C2262">
-        <v>6369</v>
+        <v>7251.6</v>
       </c>
       <c r="D2262" t="s">
         <v>2264</v>
@@ -40133,7 +40133,7 @@
         <v>54</v>
       </c>
       <c r="C2263">
-        <v>6292.5</v>
+        <v>7253.9</v>
       </c>
       <c r="D2263" t="s">
         <v>2265</v>
@@ -40147,7 +40147,7 @@
         <v>55</v>
       </c>
       <c r="C2264">
-        <v>6262.6</v>
+        <v>7306.1</v>
       </c>
       <c r="D2264" t="s">
         <v>2266</v>
@@ -40161,7 +40161,7 @@
         <v>56</v>
       </c>
       <c r="C2265">
-        <v>6248.6</v>
+        <v>7348.9</v>
       </c>
       <c r="D2265" t="s">
         <v>2267</v>
@@ -40175,7 +40175,7 @@
         <v>57</v>
       </c>
       <c r="C2266">
-        <v>6522</v>
+        <v>7441.9</v>
       </c>
       <c r="D2266" t="s">
         <v>2268</v>
@@ -40189,7 +40189,7 @@
         <v>58</v>
       </c>
       <c r="C2267">
-        <v>6460</v>
+        <v>7443.3</v>
       </c>
       <c r="D2267" t="s">
         <v>2269</v>
@@ -40203,7 +40203,7 @@
         <v>59</v>
       </c>
       <c r="C2268">
-        <v>6409.9</v>
+        <v>7435.1</v>
       </c>
       <c r="D2268" t="s">
         <v>2270</v>
@@ -40217,7 +40217,7 @@
         <v>60</v>
       </c>
       <c r="C2269">
-        <v>6343</v>
+        <v>7442.8</v>
       </c>
       <c r="D2269" t="s">
         <v>2271</v>
@@ -40231,7 +40231,7 @@
         <v>61</v>
       </c>
       <c r="C2270">
-        <v>6478.9</v>
+        <v>7595</v>
       </c>
       <c r="D2270" t="s">
         <v>2272</v>
@@ -40245,7 +40245,7 @@
         <v>62</v>
       </c>
       <c r="C2271">
-        <v>6443.4</v>
+        <v>7530.6</v>
       </c>
       <c r="D2271" t="s">
         <v>2273</v>
@@ -40259,7 +40259,7 @@
         <v>63</v>
       </c>
       <c r="C2272">
-        <v>6438.6</v>
+        <v>7484.4</v>
       </c>
       <c r="D2272" t="s">
         <v>2274</v>
@@ -40273,7 +40273,7 @@
         <v>64</v>
       </c>
       <c r="C2273">
-        <v>6397.6</v>
+        <v>7425.6</v>
       </c>
       <c r="D2273" t="s">
         <v>2275</v>
@@ -40287,7 +40287,7 @@
         <v>65</v>
       </c>
       <c r="C2274">
-        <v>6632.4</v>
+        <v>7893.1</v>
       </c>
       <c r="D2274" t="s">
         <v>2276</v>
@@ -40301,7 +40301,7 @@
         <v>66</v>
       </c>
       <c r="C2275">
-        <v>6647.4</v>
+        <v>7891.6</v>
       </c>
       <c r="D2275" t="s">
         <v>2277</v>
@@ -40315,7 +40315,7 @@
         <v>67</v>
       </c>
       <c r="C2276">
-        <v>6666.4</v>
+        <v>7896</v>
       </c>
       <c r="D2276" t="s">
         <v>2278</v>
@@ -40329,7 +40329,7 @@
         <v>68</v>
       </c>
       <c r="C2277">
-        <v>6715.2</v>
+        <v>7895.5</v>
       </c>
       <c r="D2277" t="s">
         <v>2279</v>
@@ -40343,7 +40343,7 @@
         <v>69</v>
       </c>
       <c r="C2278">
-        <v>6832.7</v>
+        <v>7870</v>
       </c>
       <c r="D2278" t="s">
         <v>2280</v>
@@ -40357,7 +40357,7 @@
         <v>70</v>
       </c>
       <c r="C2279">
-        <v>6920.1</v>
+        <v>7870.5</v>
       </c>
       <c r="D2279" t="s">
         <v>2281</v>
@@ -40371,7 +40371,7 @@
         <v>71</v>
       </c>
       <c r="C2280">
-        <v>6935.6</v>
+        <v>7893</v>
       </c>
       <c r="D2280" t="s">
         <v>2282</v>
@@ -40385,7 +40385,7 @@
         <v>72</v>
       </c>
       <c r="C2281">
-        <v>7003.7</v>
+        <v>7893.9</v>
       </c>
       <c r="D2281" t="s">
         <v>2283</v>
@@ -40399,7 +40399,7 @@
         <v>73</v>
       </c>
       <c r="C2282">
-        <v>7300.4</v>
+        <v>8229.799999999999</v>
       </c>
       <c r="D2282" t="s">
         <v>2284</v>
@@ -40413,7 +40413,7 @@
         <v>74</v>
       </c>
       <c r="C2283">
-        <v>7363.9</v>
+        <v>8211.1</v>
       </c>
       <c r="D2283" t="s">
         <v>2285</v>
@@ -40427,7 +40427,7 @@
         <v>75</v>
       </c>
       <c r="C2284">
-        <v>7464.2</v>
+        <v>8245.700000000001</v>
       </c>
       <c r="D2284" t="s">
         <v>2286</v>
@@ -40441,7 +40441,7 @@
         <v>76</v>
       </c>
       <c r="C2285">
-        <v>7572.7</v>
+        <v>8288.6</v>
       </c>
       <c r="D2285" t="s">
         <v>2287</v>
@@ -40455,7 +40455,7 @@
         <v>77</v>
       </c>
       <c r="C2286">
-        <v>7770.6</v>
+        <v>8373.6</v>
       </c>
       <c r="D2286" t="s">
         <v>2288</v>
@@ -40469,7 +40469,7 @@
         <v>78</v>
       </c>
       <c r="C2287">
-        <v>7888.6</v>
+        <v>8440.299999999999</v>
       </c>
       <c r="D2287" t="s">
         <v>2289</v>
@@ -40483,7 +40483,7 @@
         <v>79</v>
       </c>
       <c r="C2288">
-        <v>7910.8</v>
+        <v>8496</v>
       </c>
       <c r="D2288" t="s">
         <v>2290</v>
@@ -40497,7 +40497,7 @@
         <v>80</v>
       </c>
       <c r="C2289">
-        <v>7974.1</v>
+        <v>8534.9</v>
       </c>
       <c r="D2289" t="s">
         <v>2291</v>
@@ -40511,7 +40511,7 @@
         <v>81</v>
       </c>
       <c r="C2290">
-        <v>7908.7</v>
+        <v>8263.9</v>
       </c>
       <c r="D2290" t="s">
         <v>2292</v>
@@ -40525,7 +40525,7 @@
         <v>82</v>
       </c>
       <c r="C2291">
-        <v>7957.2</v>
+        <v>8298.1</v>
       </c>
       <c r="D2291" t="s">
         <v>2293</v>
@@ -40539,7 +40539,7 @@
         <v>83</v>
       </c>
       <c r="C2292">
-        <v>7932.5</v>
+        <v>8350.299999999999</v>
       </c>
       <c r="D2292" t="s">
         <v>2294</v>
@@ -40553,7 +40553,7 @@
         <v>84</v>
       </c>
       <c r="C2293">
-        <v>7937.2</v>
+        <v>8395.299999999999</v>
       </c>
       <c r="D2293" t="s">
         <v>2295</v>
@@ -40567,7 +40567,7 @@
         <v>85</v>
       </c>
       <c r="C2294">
-        <v>8071.4</v>
+        <v>8274.799999999999</v>
       </c>
       <c r="D2294" t="s">
         <v>2296</v>
@@ -40581,7 +40581,7 @@
         <v>86</v>
       </c>
       <c r="C2295">
-        <v>8011.8</v>
+        <v>8226.700000000001</v>
       </c>
       <c r="D2295" t="s">
         <v>2297</v>
@@ -40595,7 +40595,7 @@
         <v>87</v>
       </c>
       <c r="C2296">
-        <v>8020.7</v>
+        <v>8225.200000000001</v>
       </c>
       <c r="D2296" t="s">
         <v>2298</v>
@@ -40609,7 +40609,7 @@
         <v>88</v>
       </c>
       <c r="C2297">
-        <v>8028.2</v>
+        <v>8224.1</v>
       </c>
       <c r="D2297" t="s">
         <v>2299</v>
@@ -40623,7 +40623,7 @@
         <v>89</v>
       </c>
       <c r="C2298">
-        <v>8111.2</v>
+        <v>8205.5</v>
       </c>
       <c r="D2298" t="s">
         <v>2300</v>
@@ -40637,7 +40637,7 @@
         <v>90</v>
       </c>
       <c r="C2299">
-        <v>8099.1</v>
+        <v>8181.7</v>
       </c>
       <c r="D2299" t="s">
         <v>2301</v>
@@ -40651,7 +40651,7 @@
         <v>91</v>
       </c>
       <c r="C2300">
-        <v>8037.1</v>
+        <v>8111</v>
       </c>
       <c r="D2300" t="s">
         <v>2302</v>
@@ -40665,7 +40665,7 @@
         <v>92</v>
       </c>
       <c r="C2301">
-        <v>7966.2</v>
+        <v>8108.7</v>
       </c>
       <c r="D2301" t="s">
         <v>2303</v>
@@ -40679,7 +40679,7 @@
         <v>93</v>
       </c>
       <c r="C2302">
-        <v>7890.6</v>
+        <v>8089.8</v>
       </c>
       <c r="D2302" t="s">
         <v>2304</v>
@@ -40693,7 +40693,7 @@
         <v>94</v>
       </c>
       <c r="C2303">
-        <v>7765.6</v>
+        <v>8046.7</v>
       </c>
       <c r="D2303" t="s">
         <v>2305</v>
@@ -40707,7 +40707,7 @@
         <v>95</v>
       </c>
       <c r="C2304">
-        <v>7737.2</v>
+        <v>8008.9</v>
       </c>
       <c r="D2304" t="s">
         <v>2306</v>
@@ -40721,7 +40721,7 @@
         <v>96</v>
       </c>
       <c r="C2305">
-        <v>7754</v>
+        <v>7985</v>
       </c>
       <c r="D2305" t="s">
         <v>2307</v>
@@ -40735,7 +40735,7 @@
         <v>1</v>
       </c>
       <c r="C2306">
-        <v>6502.2</v>
+        <v>6182</v>
       </c>
       <c r="D2306" t="s">
         <v>2308</v>
@@ -40749,7 +40749,7 @@
         <v>2</v>
       </c>
       <c r="C2307">
-        <v>6476.3</v>
+        <v>6132</v>
       </c>
       <c r="D2307" t="s">
         <v>2309</v>
@@ -40763,7 +40763,7 @@
         <v>3</v>
       </c>
       <c r="C2308">
-        <v>6454.1</v>
+        <v>6082</v>
       </c>
       <c r="D2308" t="s">
         <v>2310</v>
@@ -40777,7 +40777,7 @@
         <v>4</v>
       </c>
       <c r="C2309">
-        <v>6362</v>
+        <v>6032</v>
       </c>
       <c r="D2309" t="s">
         <v>2311</v>
@@ -40791,7 +40791,7 @@
         <v>5</v>
       </c>
       <c r="C2310">
-        <v>7019</v>
+        <v>6026</v>
       </c>
       <c r="D2310" t="s">
         <v>2312</v>
@@ -40805,7 +40805,7 @@
         <v>6</v>
       </c>
       <c r="C2311">
-        <v>6925</v>
+        <v>6001</v>
       </c>
       <c r="D2311" t="s">
         <v>2313</v>
@@ -40819,7 +40819,7 @@
         <v>7</v>
       </c>
       <c r="C2312">
-        <v>6915.1</v>
+        <v>5945.8</v>
       </c>
       <c r="D2312" t="s">
         <v>2314</v>
@@ -40833,7 +40833,7 @@
         <v>8</v>
       </c>
       <c r="C2313">
-        <v>6865.6</v>
+        <v>5906.7</v>
       </c>
       <c r="D2313" t="s">
         <v>2315</v>
@@ -40847,7 +40847,7 @@
         <v>9</v>
       </c>
       <c r="C2314">
-        <v>6708.2</v>
+        <v>5895.2</v>
       </c>
       <c r="D2314" t="s">
         <v>2316</v>
@@ -40861,7 +40861,7 @@
         <v>10</v>
       </c>
       <c r="C2315">
-        <v>6714.7</v>
+        <v>5852.5</v>
       </c>
       <c r="D2315" t="s">
         <v>2317</v>
@@ -40875,7 +40875,7 @@
         <v>11</v>
       </c>
       <c r="C2316">
-        <v>6704.6</v>
+        <v>5877.3</v>
       </c>
       <c r="D2316" t="s">
         <v>2318</v>
@@ -40889,7 +40889,7 @@
         <v>12</v>
       </c>
       <c r="C2317">
-        <v>6688.4</v>
+        <v>5843.7</v>
       </c>
       <c r="D2317" t="s">
         <v>2319</v>
@@ -40903,7 +40903,7 @@
         <v>13</v>
       </c>
       <c r="C2318">
-        <v>6487.2</v>
+        <v>5914.3</v>
       </c>
       <c r="D2318" t="s">
         <v>2320</v>
@@ -40917,7 +40917,7 @@
         <v>14</v>
       </c>
       <c r="C2319">
-        <v>6488.6</v>
+        <v>5917.8</v>
       </c>
       <c r="D2319" t="s">
         <v>2321</v>
@@ -40931,7 +40931,7 @@
         <v>15</v>
       </c>
       <c r="C2320">
-        <v>6464.5</v>
+        <v>5922.4</v>
       </c>
       <c r="D2320" t="s">
         <v>2322</v>
@@ -40945,7 +40945,7 @@
         <v>16</v>
       </c>
       <c r="C2321">
-        <v>6460.9</v>
+        <v>5927.9</v>
       </c>
       <c r="D2321" t="s">
         <v>2323</v>
@@ -40959,7 +40959,7 @@
         <v>17</v>
       </c>
       <c r="C2322">
-        <v>6450.7</v>
+        <v>5896.8</v>
       </c>
       <c r="D2322" t="s">
         <v>2324</v>
@@ -40973,7 +40973,7 @@
         <v>18</v>
       </c>
       <c r="C2323">
-        <v>6474.4</v>
+        <v>5903.9</v>
       </c>
       <c r="D2323" t="s">
         <v>2325</v>
@@ -40987,7 +40987,7 @@
         <v>19</v>
       </c>
       <c r="C2324">
-        <v>6500.5</v>
+        <v>5894.1</v>
       </c>
       <c r="D2324" t="s">
         <v>2326</v>
@@ -41001,7 +41001,7 @@
         <v>20</v>
       </c>
       <c r="C2325">
-        <v>6530.7</v>
+        <v>5897.9</v>
       </c>
       <c r="D2325" t="s">
         <v>2327</v>
@@ -41015,7 +41015,7 @@
         <v>21</v>
       </c>
       <c r="C2326">
-        <v>6529.9</v>
+        <v>5826.6</v>
       </c>
       <c r="D2326" t="s">
         <v>2328</v>
@@ -41029,7 +41029,7 @@
         <v>22</v>
       </c>
       <c r="C2327">
-        <v>6580.4</v>
+        <v>5849.9</v>
       </c>
       <c r="D2327" t="s">
         <v>2329</v>
@@ -41043,7 +41043,7 @@
         <v>23</v>
       </c>
       <c r="C2328">
-        <v>6624</v>
+        <v>5874.8</v>
       </c>
       <c r="D2328" t="s">
         <v>2330</v>
@@ -41057,7 +41057,7 @@
         <v>24</v>
       </c>
       <c r="C2329">
-        <v>6655.2</v>
+        <v>5882.9</v>
       </c>
       <c r="D2329" t="s">
         <v>2331</v>
@@ -41071,7 +41071,7 @@
         <v>25</v>
       </c>
       <c r="C2330">
-        <v>6981.3</v>
+        <v>5907.8</v>
       </c>
       <c r="D2330" t="s">
         <v>2332</v>
@@ -41085,7 +41085,7 @@
         <v>26</v>
       </c>
       <c r="C2331">
-        <v>6984.8</v>
+        <v>6001.2</v>
       </c>
       <c r="D2331" t="s">
         <v>2333</v>
@@ -41099,7 +41099,7 @@
         <v>27</v>
       </c>
       <c r="C2332">
-        <v>7034.4</v>
+        <v>6108.7</v>
       </c>
       <c r="D2332" t="s">
         <v>2334</v>
@@ -41113,7 +41113,7 @@
         <v>28</v>
       </c>
       <c r="C2333">
-        <v>7049.6</v>
+        <v>6181</v>
       </c>
       <c r="D2333" t="s">
         <v>2335</v>
@@ -41127,7 +41127,7 @@
         <v>29</v>
       </c>
       <c r="C2334">
-        <v>7399.9</v>
+        <v>6878.9</v>
       </c>
       <c r="D2334" t="s">
         <v>2336</v>
@@ -41141,7 +41141,7 @@
         <v>30</v>
       </c>
       <c r="C2335">
-        <v>7441</v>
+        <v>6920.9</v>
       </c>
       <c r="D2335" t="s">
         <v>2337</v>
@@ -41155,7 +41155,7 @@
         <v>31</v>
       </c>
       <c r="C2336">
-        <v>7526.1</v>
+        <v>7049.7</v>
       </c>
       <c r="D2336" t="s">
         <v>2338</v>
@@ -41169,7 +41169,7 @@
         <v>32</v>
       </c>
       <c r="C2337">
-        <v>7576.9</v>
+        <v>7097.6</v>
       </c>
       <c r="D2337" t="s">
         <v>2339</v>
@@ -41183,7 +41183,7 @@
         <v>33</v>
       </c>
       <c r="C2338">
-        <v>7388.9</v>
+        <v>7005.7</v>
       </c>
       <c r="D2338" t="s">
         <v>2340</v>
@@ -41197,7 +41197,7 @@
         <v>34</v>
       </c>
       <c r="C2339">
-        <v>7502</v>
+        <v>7045.4</v>
       </c>
       <c r="D2339" t="s">
         <v>2341</v>
@@ -41211,7 +41211,7 @@
         <v>35</v>
       </c>
       <c r="C2340">
-        <v>7580.5</v>
+        <v>7034.1</v>
       </c>
       <c r="D2340" t="s">
         <v>2342</v>
@@ -41225,7 +41225,7 @@
         <v>36</v>
       </c>
       <c r="C2341">
-        <v>7619.7</v>
+        <v>7067.3</v>
       </c>
       <c r="D2341" t="s">
         <v>2343</v>
@@ -41239,7 +41239,7 @@
         <v>37</v>
       </c>
       <c r="C2342">
-        <v>7337.6</v>
+        <v>6932.8</v>
       </c>
       <c r="D2342" t="s">
         <v>2344</v>
@@ -41253,7 +41253,7 @@
         <v>38</v>
       </c>
       <c r="C2343">
-        <v>7342.2</v>
+        <v>6888.8</v>
       </c>
       <c r="D2343" t="s">
         <v>2345</v>
@@ -41267,7 +41267,7 @@
         <v>39</v>
       </c>
       <c r="C2344">
-        <v>7370.5</v>
+        <v>6865.1</v>
       </c>
       <c r="D2344" t="s">
         <v>2346</v>
@@ -41281,7 +41281,7 @@
         <v>40</v>
       </c>
       <c r="C2345">
-        <v>7370.2</v>
+        <v>6828</v>
       </c>
       <c r="D2345" t="s">
         <v>2347</v>
@@ -41295,7 +41295,7 @@
         <v>41</v>
       </c>
       <c r="C2346">
-        <v>6754.9</v>
+        <v>6754.4</v>
       </c>
       <c r="D2346" t="s">
         <v>2348</v>
@@ -41309,7 +41309,7 @@
         <v>42</v>
       </c>
       <c r="C2347">
-        <v>6734.7</v>
+        <v>6738.5</v>
       </c>
       <c r="D2347" t="s">
         <v>2349</v>
@@ -41323,7 +41323,7 @@
         <v>43</v>
       </c>
       <c r="C2348">
-        <v>6743.5</v>
+        <v>6740.1</v>
       </c>
       <c r="D2348" t="s">
         <v>2350</v>
@@ -41337,7 +41337,7 @@
         <v>44</v>
       </c>
       <c r="C2349">
-        <v>6763.2</v>
+        <v>6747.8</v>
       </c>
       <c r="D2349" t="s">
         <v>2351</v>
@@ -41351,7 +41351,7 @@
         <v>45</v>
       </c>
       <c r="C2350">
-        <v>7013.1</v>
+        <v>6380.9</v>
       </c>
       <c r="D2350" t="s">
         <v>2352</v>
@@ -41365,7 +41365,7 @@
         <v>46</v>
       </c>
       <c r="C2351">
-        <v>6999.6</v>
+        <v>6405.6</v>
       </c>
       <c r="D2351" t="s">
         <v>2353</v>
@@ -41379,7 +41379,7 @@
         <v>47</v>
       </c>
       <c r="C2352">
-        <v>7002.8</v>
+        <v>6424.3</v>
       </c>
       <c r="D2352" t="s">
         <v>2354</v>
@@ -41393,7 +41393,7 @@
         <v>48</v>
       </c>
       <c r="C2353">
-        <v>7011.7</v>
+        <v>6465.4</v>
       </c>
       <c r="D2353" t="s">
         <v>2355</v>
@@ -41407,7 +41407,7 @@
         <v>49</v>
       </c>
       <c r="C2354">
-        <v>6797.7</v>
+        <v>6483</v>
       </c>
       <c r="D2354" t="s">
         <v>2356</v>
@@ -41421,7 +41421,7 @@
         <v>50</v>
       </c>
       <c r="C2355">
-        <v>6799.4</v>
+        <v>6538</v>
       </c>
       <c r="D2355" t="s">
         <v>2357</v>
@@ -41435,7 +41435,7 @@
         <v>51</v>
       </c>
       <c r="C2356">
-        <v>6777.7</v>
+        <v>6574.6</v>
       </c>
       <c r="D2356" t="s">
         <v>2358</v>
@@ -41449,7 +41449,7 @@
         <v>52</v>
       </c>
       <c r="C2357">
-        <v>6738</v>
+        <v>6639.2</v>
       </c>
       <c r="D2357" t="s">
         <v>2359</v>
@@ -41463,7 +41463,7 @@
         <v>53</v>
       </c>
       <c r="C2358">
-        <v>6599</v>
+        <v>6611.6</v>
       </c>
       <c r="D2358" t="s">
         <v>2360</v>
@@ -41477,7 +41477,7 @@
         <v>54</v>
       </c>
       <c r="C2359">
-        <v>6522.5</v>
+        <v>6613.9</v>
       </c>
       <c r="D2359" t="s">
         <v>2361</v>
@@ -41491,7 +41491,7 @@
         <v>55</v>
       </c>
       <c r="C2360">
-        <v>6492.6</v>
+        <v>6676.1</v>
       </c>
       <c r="D2360" t="s">
         <v>2362</v>
@@ -41505,7 +41505,7 @@
         <v>56</v>
       </c>
       <c r="C2361">
-        <v>6478.6</v>
+        <v>6738.9</v>
       </c>
       <c r="D2361" t="s">
         <v>2363</v>
@@ -41519,7 +41519,7 @@
         <v>57</v>
       </c>
       <c r="C2362">
-        <v>6742</v>
+        <v>6851.9</v>
       </c>
       <c r="D2362" t="s">
         <v>2364</v>
@@ -41533,7 +41533,7 @@
         <v>58</v>
       </c>
       <c r="C2363">
-        <v>6680</v>
+        <v>6853.3</v>
       </c>
       <c r="D2363" t="s">
         <v>2365</v>
@@ -41547,7 +41547,7 @@
         <v>59</v>
       </c>
       <c r="C2364">
-        <v>6619.9</v>
+        <v>6855.1</v>
       </c>
       <c r="D2364" t="s">
         <v>2366</v>
@@ -41561,7 +41561,7 @@
         <v>60</v>
       </c>
       <c r="C2365">
-        <v>6553</v>
+        <v>6882.8</v>
       </c>
       <c r="D2365" t="s">
         <v>2367</v>
@@ -41575,7 +41575,7 @@
         <v>61</v>
       </c>
       <c r="C2366">
-        <v>6678.9</v>
+        <v>7065</v>
       </c>
       <c r="D2366" t="s">
         <v>2368</v>
@@ -41589,7 +41589,7 @@
         <v>62</v>
       </c>
       <c r="C2367">
-        <v>6623.4</v>
+        <v>7020.6</v>
       </c>
       <c r="D2367" t="s">
         <v>2369</v>
@@ -41603,7 +41603,7 @@
         <v>63</v>
       </c>
       <c r="C2368">
-        <v>6618.6</v>
+        <v>7014.4</v>
       </c>
       <c r="D2368" t="s">
         <v>2370</v>
@@ -41617,7 +41617,7 @@
         <v>64</v>
       </c>
       <c r="C2369">
-        <v>6547.6</v>
+        <v>7005.6</v>
       </c>
       <c r="D2369" t="s">
         <v>2371</v>
@@ -41631,7 +41631,7 @@
         <v>65</v>
       </c>
       <c r="C2370">
-        <v>6772.4</v>
+        <v>7503.1</v>
       </c>
       <c r="D2370" t="s">
         <v>2372</v>
@@ -41645,7 +41645,7 @@
         <v>66</v>
       </c>
       <c r="C2371">
-        <v>6757.4</v>
+        <v>7551.6</v>
       </c>
       <c r="D2371" t="s">
         <v>2373</v>
@@ -41659,7 +41659,7 @@
         <v>67</v>
       </c>
       <c r="C2372">
-        <v>6756.4</v>
+        <v>7606</v>
       </c>
       <c r="D2372" t="s">
         <v>2374</v>
@@ -41673,7 +41673,7 @@
         <v>68</v>
       </c>
       <c r="C2373">
-        <v>6775.2</v>
+        <v>7655.5</v>
       </c>
       <c r="D2373" t="s">
         <v>2375</v>
@@ -41687,7 +41687,7 @@
         <v>69</v>
       </c>
       <c r="C2374">
-        <v>6862.7</v>
+        <v>7700</v>
       </c>
       <c r="D2374" t="s">
         <v>2376</v>
@@ -41701,7 +41701,7 @@
         <v>70</v>
       </c>
       <c r="C2375">
-        <v>6920.1</v>
+        <v>7750.5</v>
       </c>
       <c r="D2375" t="s">
         <v>2377</v>
@@ -41715,7 +41715,7 @@
         <v>71</v>
       </c>
       <c r="C2376">
-        <v>6915.6</v>
+        <v>7813</v>
       </c>
       <c r="D2376" t="s">
         <v>2378</v>
@@ -41729,7 +41729,7 @@
         <v>72</v>
       </c>
       <c r="C2377">
-        <v>6953.7</v>
+        <v>7833.9</v>
       </c>
       <c r="D2377" t="s">
         <v>2379</v>
@@ -41743,7 +41743,7 @@
         <v>73</v>
       </c>
       <c r="C2378">
-        <v>7230.4</v>
+        <v>8179.8</v>
       </c>
       <c r="D2378" t="s">
         <v>2380</v>
@@ -41757,7 +41757,7 @@
         <v>74</v>
       </c>
       <c r="C2379">
-        <v>7273.9</v>
+        <v>8181.1</v>
       </c>
       <c r="D2379" t="s">
         <v>2381</v>
@@ -41771,7 +41771,7 @@
         <v>75</v>
       </c>
       <c r="C2380">
-        <v>7364.2</v>
+        <v>8245.700000000001</v>
       </c>
       <c r="D2380" t="s">
         <v>2382</v>
@@ -41785,7 +41785,7 @@
         <v>76</v>
       </c>
       <c r="C2381">
-        <v>7472.7</v>
+        <v>8318.6</v>
       </c>
       <c r="D2381" t="s">
         <v>2383</v>
@@ -41799,7 +41799,7 @@
         <v>77</v>
       </c>
       <c r="C2382">
-        <v>7670.6</v>
+        <v>8433.6</v>
       </c>
       <c r="D2382" t="s">
         <v>2384</v>
@@ -41813,7 +41813,7 @@
         <v>78</v>
       </c>
       <c r="C2383">
-        <v>7798.6</v>
+        <v>8540.299999999999</v>
       </c>
       <c r="D2383" t="s">
         <v>2385</v>
@@ -41827,7 +41827,7 @@
         <v>79</v>
       </c>
       <c r="C2384">
-        <v>7820.8</v>
+        <v>8616</v>
       </c>
       <c r="D2384" t="s">
         <v>2386</v>
@@ -41841,7 +41841,7 @@
         <v>80</v>
       </c>
       <c r="C2385">
-        <v>7884.1</v>
+        <v>8684.9</v>
       </c>
       <c r="D2385" t="s">
         <v>2387</v>
@@ -41855,7 +41855,7 @@
         <v>81</v>
       </c>
       <c r="C2386">
-        <v>7828.7</v>
+        <v>8443.9</v>
       </c>
       <c r="D2386" t="s">
         <v>2388</v>
@@ -41869,7 +41869,7 @@
         <v>82</v>
       </c>
       <c r="C2387">
-        <v>7867.2</v>
+        <v>8468.1</v>
       </c>
       <c r="D2387" t="s">
         <v>2389</v>
@@ -41883,7 +41883,7 @@
         <v>83</v>
       </c>
       <c r="C2388">
-        <v>7852.5</v>
+        <v>8500.299999999999</v>
       </c>
       <c r="D2388" t="s">
         <v>2390</v>
@@ -41897,7 +41897,7 @@
         <v>84</v>
       </c>
       <c r="C2389">
-        <v>7857.2</v>
+        <v>8555.299999999999</v>
       </c>
       <c r="D2389" t="s">
         <v>2391</v>
@@ -41911,7 +41911,7 @@
         <v>85</v>
       </c>
       <c r="C2390">
-        <v>7991.4</v>
+        <v>8414.799999999999</v>
       </c>
       <c r="D2390" t="s">
         <v>2392</v>
@@ -41925,7 +41925,7 @@
         <v>86</v>
       </c>
       <c r="C2391">
-        <v>7931.8</v>
+        <v>8346.700000000001</v>
       </c>
       <c r="D2391" t="s">
         <v>2393</v>
@@ -41939,7 +41939,7 @@
         <v>87</v>
       </c>
       <c r="C2392">
-        <v>7940.7</v>
+        <v>8335.200000000001</v>
       </c>
       <c r="D2392" t="s">
         <v>2394</v>
@@ -41953,7 +41953,7 @@
         <v>88</v>
       </c>
       <c r="C2393">
-        <v>7948.2</v>
+        <v>8334.1</v>
       </c>
       <c r="D2393" t="s">
         <v>2395</v>
@@ -41967,7 +41967,7 @@
         <v>89</v>
       </c>
       <c r="C2394">
-        <v>8031.2</v>
+        <v>8325.5</v>
       </c>
       <c r="D2394" t="s">
         <v>2396</v>
@@ -41981,7 +41981,7 @@
         <v>90</v>
       </c>
       <c r="C2395">
-        <v>8019.1</v>
+        <v>8301.700000000001</v>
       </c>
       <c r="D2395" t="s">
         <v>2397</v>
@@ -41995,7 +41995,7 @@
         <v>91</v>
       </c>
       <c r="C2396">
-        <v>7957.1</v>
+        <v>8201</v>
       </c>
       <c r="D2396" t="s">
         <v>2398</v>
@@ -42009,7 +42009,7 @@
         <v>92</v>
       </c>
       <c r="C2397">
-        <v>7886.2</v>
+        <v>8208.700000000001</v>
       </c>
       <c r="D2397" t="s">
         <v>2399</v>
@@ -42023,7 +42023,7 @@
         <v>93</v>
       </c>
       <c r="C2398">
-        <v>7810.6</v>
+        <v>8169.8</v>
       </c>
       <c r="D2398" t="s">
         <v>2400</v>
@@ -42037,7 +42037,7 @@
         <v>94</v>
       </c>
       <c r="C2399">
-        <v>7685.6</v>
+        <v>8076.7</v>
       </c>
       <c r="D2399" t="s">
         <v>2401</v>
@@ -42051,7 +42051,7 @@
         <v>95</v>
       </c>
       <c r="C2400">
-        <v>7657.2</v>
+        <v>8058.9</v>
       </c>
       <c r="D2400" t="s">
         <v>2402</v>
@@ -42065,7 +42065,7 @@
         <v>96</v>
       </c>
       <c r="C2401">
-        <v>7674</v>
+        <v>8035</v>
       </c>
       <c r="D2401" t="s">
         <v>2403</v>
@@ -42079,7 +42079,7 @@
         <v>1</v>
       </c>
       <c r="C2402">
-        <v>6452.2</v>
+        <v>6282</v>
       </c>
       <c r="D2402" t="s">
         <v>2404</v>
@@ -42093,7 +42093,7 @@
         <v>2</v>
       </c>
       <c r="C2403">
-        <v>6406.3</v>
+        <v>6242</v>
       </c>
       <c r="D2403" t="s">
         <v>2405</v>
@@ -42107,7 +42107,7 @@
         <v>3</v>
       </c>
       <c r="C2404">
-        <v>6374.1</v>
+        <v>6182</v>
       </c>
       <c r="D2404" t="s">
         <v>2406</v>
@@ -42121,7 +42121,7 @@
         <v>4</v>
       </c>
       <c r="C2405">
-        <v>6292</v>
+        <v>6122</v>
       </c>
       <c r="D2405" t="s">
         <v>2407</v>
@@ -42135,7 +42135,7 @@
         <v>5</v>
       </c>
       <c r="C2406">
-        <v>6969</v>
+        <v>6126</v>
       </c>
       <c r="D2406" t="s">
         <v>2408</v>
@@ -42149,7 +42149,7 @@
         <v>6</v>
       </c>
       <c r="C2407">
-        <v>6875</v>
+        <v>6101</v>
       </c>
       <c r="D2407" t="s">
         <v>2409</v>
@@ -42163,7 +42163,7 @@
         <v>7</v>
       </c>
       <c r="C2408">
-        <v>6865.1</v>
+        <v>6055.8</v>
       </c>
       <c r="D2408" t="s">
         <v>2410</v>
@@ -42177,7 +42177,7 @@
         <v>8</v>
       </c>
       <c r="C2409">
-        <v>6825.6</v>
+        <v>6016.7</v>
       </c>
       <c r="D2409" t="s">
         <v>2411</v>
@@ -42191,7 +42191,7 @@
         <v>9</v>
       </c>
       <c r="C2410">
-        <v>6648.2</v>
+        <v>5995.2</v>
       </c>
       <c r="D2410" t="s">
         <v>2412</v>
@@ -42205,7 +42205,7 @@
         <v>10</v>
       </c>
       <c r="C2411">
-        <v>6664.7</v>
+        <v>5962.5</v>
       </c>
       <c r="D2411" t="s">
         <v>2413</v>
@@ -42219,7 +42219,7 @@
         <v>11</v>
       </c>
       <c r="C2412">
-        <v>6644.6</v>
+        <v>5977.3</v>
       </c>
       <c r="D2412" t="s">
         <v>2414</v>
@@ -42233,7 +42233,7 @@
         <v>12</v>
       </c>
       <c r="C2413">
-        <v>6628.4</v>
+        <v>5943.7</v>
       </c>
       <c r="D2413" t="s">
         <v>2415</v>
@@ -42247,7 +42247,7 @@
         <v>13</v>
       </c>
       <c r="C2414">
-        <v>6427.2</v>
+        <v>6014.3</v>
       </c>
       <c r="D2414" t="s">
         <v>2416</v>
@@ -42261,7 +42261,7 @@
         <v>14</v>
       </c>
       <c r="C2415">
-        <v>6418.6</v>
+        <v>6017.8</v>
       </c>
       <c r="D2415" t="s">
         <v>2417</v>
@@ -42275,7 +42275,7 @@
         <v>15</v>
       </c>
       <c r="C2416">
-        <v>6404.5</v>
+        <v>6022.4</v>
       </c>
       <c r="D2416" t="s">
         <v>2418</v>
@@ -42289,7 +42289,7 @@
         <v>16</v>
       </c>
       <c r="C2417">
-        <v>6400.9</v>
+        <v>6027.9</v>
       </c>
       <c r="D2417" t="s">
         <v>2419</v>
@@ -42303,7 +42303,7 @@
         <v>17</v>
       </c>
       <c r="C2418">
-        <v>6390.7</v>
+        <v>5996.8</v>
       </c>
       <c r="D2418" t="s">
         <v>2420</v>
@@ -42317,7 +42317,7 @@
         <v>18</v>
       </c>
       <c r="C2419">
-        <v>6414.4</v>
+        <v>6003.9</v>
       </c>
       <c r="D2419" t="s">
         <v>2421</v>
@@ -42331,7 +42331,7 @@
         <v>19</v>
       </c>
       <c r="C2420">
-        <v>6430.5</v>
+        <v>5994.1</v>
       </c>
       <c r="D2420" t="s">
         <v>2422</v>
@@ -42345,7 +42345,7 @@
         <v>20</v>
       </c>
       <c r="C2421">
-        <v>6460.7</v>
+        <v>6007.9</v>
       </c>
       <c r="D2421" t="s">
         <v>2423</v>
@@ -42359,7 +42359,7 @@
         <v>21</v>
       </c>
       <c r="C2422">
-        <v>6439.9</v>
+        <v>5936.6</v>
       </c>
       <c r="D2422" t="s">
         <v>2424</v>
@@ -42373,7 +42373,7 @@
         <v>22</v>
       </c>
       <c r="C2423">
-        <v>6470.4</v>
+        <v>5959.9</v>
       </c>
       <c r="D2423" t="s">
         <v>2425</v>
@@ -42387,7 +42387,7 @@
         <v>23</v>
       </c>
       <c r="C2424">
-        <v>6514</v>
+        <v>5994.8</v>
       </c>
       <c r="D2424" t="s">
         <v>2426</v>
@@ -42401,7 +42401,7 @@
         <v>24</v>
       </c>
       <c r="C2425">
-        <v>6525.2</v>
+        <v>6002.9</v>
       </c>
       <c r="D2425" t="s">
         <v>2427</v>
@@ -42415,7 +42415,7 @@
         <v>25</v>
       </c>
       <c r="C2426">
-        <v>6841.3</v>
+        <v>6017.8</v>
       </c>
       <c r="D2426" t="s">
         <v>2428</v>
@@ -42429,7 +42429,7 @@
         <v>26</v>
       </c>
       <c r="C2427">
-        <v>6854.8</v>
+        <v>6101.2</v>
       </c>
       <c r="D2427" t="s">
         <v>2429</v>
@@ -42443,7 +42443,7 @@
         <v>27</v>
       </c>
       <c r="C2428">
-        <v>6934.4</v>
+        <v>6198.7</v>
       </c>
       <c r="D2428" t="s">
         <v>2430</v>
@@ -42457,7 +42457,7 @@
         <v>28</v>
       </c>
       <c r="C2429">
-        <v>6999.6</v>
+        <v>6251</v>
       </c>
       <c r="D2429" t="s">
         <v>2431</v>
@@ -42471,7 +42471,7 @@
         <v>29</v>
       </c>
       <c r="C2430">
-        <v>7429.9</v>
+        <v>6928.9</v>
       </c>
       <c r="D2430" t="s">
         <v>2432</v>
@@ -42485,7 +42485,7 @@
         <v>30</v>
       </c>
       <c r="C2431">
-        <v>7491</v>
+        <v>6960.9</v>
       </c>
       <c r="D2431" t="s">
         <v>2433</v>
@@ -42499,7 +42499,7 @@
         <v>31</v>
       </c>
       <c r="C2432">
-        <v>7566.1</v>
+        <v>7069.7</v>
       </c>
       <c r="D2432" t="s">
         <v>2434</v>
@@ -42513,7 +42513,7 @@
         <v>32</v>
       </c>
       <c r="C2433">
-        <v>7546.9</v>
+        <v>7097.6</v>
       </c>
       <c r="D2433" t="s">
         <v>2435</v>
@@ -42527,7 +42527,7 @@
         <v>33</v>
       </c>
       <c r="C2434">
-        <v>7268.9</v>
+        <v>6995.7</v>
       </c>
       <c r="D2434" t="s">
         <v>2436</v>
@@ -42541,7 +42541,7 @@
         <v>34</v>
       </c>
       <c r="C2435">
-        <v>7282</v>
+        <v>7025.4</v>
       </c>
       <c r="D2435" t="s">
         <v>2437</v>
@@ -42555,7 +42555,7 @@
         <v>35</v>
       </c>
       <c r="C2436">
-        <v>7280.5</v>
+        <v>7034.1</v>
       </c>
       <c r="D2436" t="s">
         <v>2438</v>
@@ -42569,7 +42569,7 @@
         <v>36</v>
       </c>
       <c r="C2437">
-        <v>7249.7</v>
+        <v>7057.3</v>
       </c>
       <c r="D2437" t="s">
         <v>2439</v>
@@ -42583,7 +42583,7 @@
         <v>37</v>
       </c>
       <c r="C2438">
-        <v>6917.6</v>
+        <v>6892.8</v>
       </c>
       <c r="D2438" t="s">
         <v>2440</v>
@@ -42597,7 +42597,7 @@
         <v>38</v>
       </c>
       <c r="C2439">
-        <v>6882.2</v>
+        <v>6828.8</v>
       </c>
       <c r="D2439" t="s">
         <v>2441</v>
@@ -42611,7 +42611,7 @@
         <v>39</v>
       </c>
       <c r="C2440">
-        <v>6880.5</v>
+        <v>6775.1</v>
       </c>
       <c r="D2440" t="s">
         <v>2442</v>
@@ -42625,7 +42625,7 @@
         <v>40</v>
       </c>
       <c r="C2441">
-        <v>6850.2</v>
+        <v>6708</v>
       </c>
       <c r="D2441" t="s">
         <v>2443</v>
@@ -42639,7 +42639,7 @@
         <v>41</v>
       </c>
       <c r="C2442">
-        <v>6204.9</v>
+        <v>6594.4</v>
       </c>
       <c r="D2442" t="s">
         <v>2444</v>
@@ -42653,7 +42653,7 @@
         <v>42</v>
       </c>
       <c r="C2443">
-        <v>6154.7</v>
+        <v>6528.5</v>
       </c>
       <c r="D2443" t="s">
         <v>2445</v>
@@ -42667,7 +42667,7 @@
         <v>43</v>
       </c>
       <c r="C2444">
-        <v>6123.5</v>
+        <v>6490.1</v>
       </c>
       <c r="D2444" t="s">
         <v>2446</v>
@@ -42681,7 +42681,7 @@
         <v>44</v>
       </c>
       <c r="C2445">
-        <v>6093.2</v>
+        <v>6467.8</v>
       </c>
       <c r="D2445" t="s">
         <v>2447</v>
@@ -42695,7 +42695,7 @@
         <v>45</v>
       </c>
       <c r="C2446">
-        <v>6283.1</v>
+        <v>6060.9</v>
       </c>
       <c r="D2446" t="s">
         <v>2448</v>
@@ -42709,7 +42709,7 @@
         <v>46</v>
       </c>
       <c r="C2447">
-        <v>6219.6</v>
+        <v>6065.6</v>
       </c>
       <c r="D2447" t="s">
         <v>2449</v>
@@ -42723,7 +42723,7 @@
         <v>47</v>
       </c>
       <c r="C2448">
-        <v>6192.8</v>
+        <v>6064.3</v>
       </c>
       <c r="D2448" t="s">
         <v>2450</v>
@@ -42737,7 +42737,7 @@
         <v>48</v>
       </c>
       <c r="C2449">
-        <v>6171.7</v>
+        <v>6095.4</v>
       </c>
       <c r="D2449" t="s">
         <v>2451</v>
@@ -42751,7 +42751,7 @@
         <v>49</v>
       </c>
       <c r="C2450">
-        <v>5947.7</v>
+        <v>6103</v>
       </c>
       <c r="D2450" t="s">
         <v>2452</v>
@@ -42765,7 +42765,7 @@
         <v>50</v>
       </c>
       <c r="C2451">
-        <v>5939.4</v>
+        <v>6148</v>
       </c>
       <c r="D2451" t="s">
         <v>2453</v>
@@ -42779,7 +42779,7 @@
         <v>51</v>
       </c>
       <c r="C2452">
-        <v>5907.7</v>
+        <v>6174.6</v>
       </c>
       <c r="D2452" t="s">
         <v>2454</v>
@@ -42793,7 +42793,7 @@
         <v>52</v>
       </c>
       <c r="C2453">
-        <v>5858</v>
+        <v>6229.2</v>
       </c>
       <c r="D2453" t="s">
         <v>2455</v>
@@ -42807,7 +42807,7 @@
         <v>53</v>
       </c>
       <c r="C2454">
-        <v>5729</v>
+        <v>6191.6</v>
       </c>
       <c r="D2454" t="s">
         <v>2456</v>
@@ -42821,7 +42821,7 @@
         <v>54</v>
       </c>
       <c r="C2455">
-        <v>5652.5</v>
+        <v>6183.9</v>
       </c>
       <c r="D2455" t="s">
         <v>2457</v>
@@ -42835,7 +42835,7 @@
         <v>55</v>
       </c>
       <c r="C2456">
-        <v>5632.6</v>
+        <v>6236.1</v>
       </c>
       <c r="D2456" t="s">
         <v>2458</v>
@@ -42849,7 +42849,7 @@
         <v>56</v>
       </c>
       <c r="C2457">
-        <v>5618.6</v>
+        <v>6288.9</v>
       </c>
       <c r="D2457" t="s">
         <v>2459</v>
@@ -42863,7 +42863,7 @@
         <v>57</v>
       </c>
       <c r="C2458">
-        <v>5902</v>
+        <v>6411.9</v>
       </c>
       <c r="D2458" t="s">
         <v>2460</v>
@@ -42877,7 +42877,7 @@
         <v>58</v>
       </c>
       <c r="C2459">
-        <v>5860</v>
+        <v>6433.3</v>
       </c>
       <c r="D2459" t="s">
         <v>2461</v>
@@ -42891,7 +42891,7 @@
         <v>59</v>
       </c>
       <c r="C2460">
-        <v>5849.9</v>
+        <v>6465.1</v>
       </c>
       <c r="D2460" t="s">
         <v>2462</v>
@@ -42905,7 +42905,7 @@
         <v>60</v>
       </c>
       <c r="C2461">
-        <v>5843</v>
+        <v>6522.8</v>
       </c>
       <c r="D2461" t="s">
         <v>2463</v>
@@ -42919,7 +42919,7 @@
         <v>61</v>
       </c>
       <c r="C2462">
-        <v>6038.9</v>
+        <v>6735</v>
       </c>
       <c r="D2462" t="s">
         <v>2464</v>
@@ -42933,7 +42933,7 @@
         <v>62</v>
       </c>
       <c r="C2463">
-        <v>6063.4</v>
+        <v>6740.6</v>
       </c>
       <c r="D2463" t="s">
         <v>2465</v>
@@ -42947,7 +42947,7 @@
         <v>63</v>
       </c>
       <c r="C2464">
-        <v>6128.6</v>
+        <v>6764.4</v>
       </c>
       <c r="D2464" t="s">
         <v>2466</v>
@@ -42961,7 +42961,7 @@
         <v>64</v>
       </c>
       <c r="C2465">
-        <v>6127.6</v>
+        <v>6775.6</v>
       </c>
       <c r="D2465" t="s">
         <v>2467</v>
@@ -42975,7 +42975,7 @@
         <v>65</v>
       </c>
       <c r="C2466">
-        <v>6402.4</v>
+        <v>7293.1</v>
       </c>
       <c r="D2466" t="s">
         <v>2468</v>
@@ -42989,7 +42989,7 @@
         <v>66</v>
       </c>
       <c r="C2467">
-        <v>6437.4</v>
+        <v>7361.6</v>
       </c>
       <c r="D2467" t="s">
         <v>2469</v>
@@ -43003,7 +43003,7 @@
         <v>67</v>
       </c>
       <c r="C2468">
-        <v>6456.4</v>
+        <v>7426</v>
       </c>
       <c r="D2468" t="s">
         <v>2470</v>
@@ -43017,7 +43017,7 @@
         <v>68</v>
       </c>
       <c r="C2469">
-        <v>6485.2</v>
+        <v>7495.5</v>
       </c>
       <c r="D2469" t="s">
         <v>2471</v>
@@ -43031,7 +43031,7 @@
         <v>69</v>
       </c>
       <c r="C2470">
-        <v>6582.7</v>
+        <v>7560</v>
       </c>
       <c r="D2470" t="s">
         <v>2472</v>
@@ -43045,7 +43045,7 @@
         <v>70</v>
       </c>
       <c r="C2471">
-        <v>6650.1</v>
+        <v>7650.5</v>
       </c>
       <c r="D2471" t="s">
         <v>2473</v>
@@ -43059,7 +43059,7 @@
         <v>71</v>
       </c>
       <c r="C2472">
-        <v>6665.6</v>
+        <v>7753</v>
       </c>
       <c r="D2472" t="s">
         <v>2474</v>
@@ -43073,7 +43073,7 @@
         <v>72</v>
       </c>
       <c r="C2473">
-        <v>6753.7</v>
+        <v>7833.9</v>
       </c>
       <c r="D2473" t="s">
         <v>2475</v>
@@ -43087,7 +43087,7 @@
         <v>73</v>
       </c>
       <c r="C2474">
-        <v>7090.4</v>
+        <v>8219.799999999999</v>
       </c>
       <c r="D2474" t="s">
         <v>2476</v>
@@ -43101,7 +43101,7 @@
         <v>74</v>
       </c>
       <c r="C2475">
-        <v>7183.9</v>
+        <v>8261.1</v>
       </c>
       <c r="D2475" t="s">
         <v>2477</v>
@@ -43115,7 +43115,7 @@
         <v>75</v>
       </c>
       <c r="C2476">
-        <v>7304.2</v>
+        <v>8355.700000000001</v>
       </c>
       <c r="D2476" t="s">
         <v>2478</v>
@@ -43129,7 +43129,7 @@
         <v>76</v>
       </c>
       <c r="C2477">
-        <v>7402.7</v>
+        <v>8448.6</v>
       </c>
       <c r="D2477" t="s">
         <v>2479</v>
@@ -43143,7 +43143,7 @@
         <v>77</v>
       </c>
       <c r="C2478">
-        <v>7580.6</v>
+        <v>8563.6</v>
       </c>
       <c r="D2478" t="s">
         <v>2480</v>
@@ -43157,7 +43157,7 @@
         <v>78</v>
       </c>
       <c r="C2479">
-        <v>7698.6</v>
+        <v>8640.299999999999</v>
       </c>
       <c r="D2479" t="s">
         <v>2481</v>
@@ -43171,7 +43171,7 @@
         <v>79</v>
       </c>
       <c r="C2480">
-        <v>7710.8</v>
+        <v>8716</v>
       </c>
       <c r="D2480" t="s">
         <v>2482</v>
@@ -43185,7 +43185,7 @@
         <v>80</v>
       </c>
       <c r="C2481">
-        <v>7774.1</v>
+        <v>8744.9</v>
       </c>
       <c r="D2481" t="s">
         <v>2483</v>
@@ -43199,7 +43199,7 @@
         <v>81</v>
       </c>
       <c r="C2482">
-        <v>7718.7</v>
+        <v>8493.9</v>
       </c>
       <c r="D2482" t="s">
         <v>2484</v>
@@ -43213,7 +43213,7 @@
         <v>82</v>
       </c>
       <c r="C2483">
-        <v>7757.2</v>
+        <v>8558.1</v>
       </c>
       <c r="D2483" t="s">
         <v>2485</v>
@@ -43227,7 +43227,7 @@
         <v>83</v>
       </c>
       <c r="C2484">
-        <v>7742.5</v>
+        <v>8600.299999999999</v>
       </c>
       <c r="D2484" t="s">
         <v>2486</v>
@@ -43241,7 +43241,7 @@
         <v>84</v>
       </c>
       <c r="C2485">
-        <v>7737.2</v>
+        <v>8645.299999999999</v>
       </c>
       <c r="D2485" t="s">
         <v>2487</v>
@@ -43255,7 +43255,7 @@
         <v>85</v>
       </c>
       <c r="C2486">
-        <v>7891.4</v>
+        <v>8504.799999999999</v>
       </c>
       <c r="D2486" t="s">
         <v>2488</v>
@@ -43269,7 +43269,7 @@
         <v>86</v>
       </c>
       <c r="C2487">
-        <v>7881.8</v>
+        <v>8456.700000000001</v>
       </c>
       <c r="D2487" t="s">
         <v>2489</v>
@@ -43283,7 +43283,7 @@
         <v>87</v>
       </c>
       <c r="C2488">
-        <v>7850.7</v>
+        <v>8435.200000000001</v>
       </c>
       <c r="D2488" t="s">
         <v>2490</v>
@@ -43297,7 +43297,7 @@
         <v>88</v>
       </c>
       <c r="C2489">
-        <v>7818.2</v>
+        <v>8444.1</v>
       </c>
       <c r="D2489" t="s">
         <v>2491</v>
@@ -43311,7 +43311,7 @@
         <v>89</v>
       </c>
       <c r="C2490">
-        <v>7901.2</v>
+        <v>8425.5</v>
       </c>
       <c r="D2490" t="s">
         <v>2492</v>
@@ -43325,7 +43325,7 @@
         <v>90</v>
       </c>
       <c r="C2491">
-        <v>7839.1</v>
+        <v>8401.700000000001</v>
       </c>
       <c r="D2491" t="s">
         <v>2493</v>
@@ -43339,7 +43339,7 @@
         <v>91</v>
       </c>
       <c r="C2492">
-        <v>7797.1</v>
+        <v>8321</v>
       </c>
       <c r="D2492" t="s">
         <v>2494</v>
@@ -43353,7 +43353,7 @@
         <v>92</v>
       </c>
       <c r="C2493">
-        <v>7746.2</v>
+        <v>8308.700000000001</v>
       </c>
       <c r="D2493" t="s">
         <v>2495</v>
@@ -43367,7 +43367,7 @@
         <v>93</v>
       </c>
       <c r="C2494">
-        <v>7730.6</v>
+        <v>8249.799999999999</v>
       </c>
       <c r="D2494" t="s">
         <v>2496</v>
@@ -43381,7 +43381,7 @@
         <v>94</v>
       </c>
       <c r="C2495">
-        <v>7675.6</v>
+        <v>8136.7</v>
       </c>
       <c r="D2495" t="s">
         <v>2497</v>
@@ -43395,7 +43395,7 @@
         <v>95</v>
       </c>
       <c r="C2496">
-        <v>7617.2</v>
+        <v>8138.9</v>
       </c>
       <c r="D2496" t="s">
         <v>2498</v>
@@ -43409,7 +43409,7 @@
         <v>96</v>
       </c>
       <c r="C2497">
-        <v>7654</v>
+        <v>8115</v>
       </c>
       <c r="D2497" t="s">
         <v>2499</v>

</xml_diff>